<commit_message>
opravena chyba ve zdroj datech "instalovany_vykon"
</commit_message>
<xml_diff>
--- a/Instalovany_vykon.xlsx
+++ b/Instalovany_vykon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LANGBRIDGE\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LANGBRIDGE\Documents\Czechitas\Projekt\Hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64458D2B-85D1-4F07-A3EF-DF258F76C647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AFF191-6476-4F6D-85DB-F8DBC5795FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{51BE5A46-95AB-422B-9A0B-CB9235A5C9FF}"/>
+    <workbookView xWindow="9675" yWindow="5355" windowWidth="19065" windowHeight="9690" xr2:uid="{51BE5A46-95AB-422B-9A0B-CB9235A5C9FF}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -311,18 +311,6 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -350,18 +338,6 @@
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -388,6 +364,30 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -8073,17 +8073,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EBEA9D-49F6-444E-A4D8-0A4D6B204266}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="10" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>2014</v>
       </c>
@@ -8112,7 +8112,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -8144,7 +8144,7 @@
         <v>20806.162549999994</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>4290</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -8208,7 +8208,7 @@
         <v>9415.8970000000008</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>1363.5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>1012.2180000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>1113.5756799999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>1171.5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>339.0949</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -8400,39 +8400,39 @@
         <v>2100.3769699999957</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>84061427.778000012</v>
+        <v>86013493.427200019</v>
       </c>
       <c r="C11" s="2">
-        <v>81801746.409999982</v>
+        <v>83893758.431299984</v>
       </c>
       <c r="D11" s="2">
-        <v>81346687.010000005</v>
+        <v>83305632.317000017</v>
       </c>
       <c r="E11" s="2">
-        <v>85019651.621999979</v>
+        <v>87041288.02699998</v>
       </c>
       <c r="F11" s="2">
-        <v>85836058.787000015</v>
+        <v>88002380.355000019</v>
       </c>
       <c r="G11" s="2">
-        <v>84878755.067000002</v>
+        <v>86991236.566000015</v>
       </c>
       <c r="H11" s="2">
-        <v>79383903.110999972</v>
+        <v>81445899.992999986</v>
       </c>
       <c r="I11" s="2">
-        <v>82931004.308999971</v>
+        <v>84907950.801999986</v>
       </c>
       <c r="J11" s="2">
-        <v>82380051.206</v>
+        <v>84503127.281000003</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
@@ -8464,7 +8464,7 @@
         <v>31021810.439999998</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>41017314.489</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>2533599.0180000002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
@@ -8560,7 +8560,7 @@
         <v>3907551.2609999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>2093465.3829999994</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
@@ -8624,7 +8624,7 @@
         <v>989708.3600000001</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>6</v>
       </c>
@@ -8656,39 +8656,39 @@
         <v>641330.47100000002</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="8">
-        <v>175271.78400000031</v>
+        <v>2127337.4332000064</v>
       </c>
       <c r="C19" s="8">
-        <v>175271.78400000031</v>
+        <v>2267283.8052999997</v>
       </c>
       <c r="D19" s="8">
-        <v>175271.78400000031</v>
+        <v>2134217.0910000028</v>
       </c>
       <c r="E19" s="8">
-        <v>175271.78400000031</v>
+        <v>2196908.1889999988</v>
       </c>
       <c r="F19" s="8">
-        <v>175271.78400000031</v>
+        <v>2341593.3519999906</v>
       </c>
       <c r="G19" s="8">
-        <v>175271.78400000031</v>
+        <v>2287753.2830000049</v>
       </c>
       <c r="H19" s="8">
-        <v>175271.78400000031</v>
+        <v>2237268.6660000025</v>
       </c>
       <c r="I19" s="8">
-        <v>175271.78400000031</v>
+        <v>2152218.2770000058</v>
       </c>
       <c r="J19" s="8">
-        <v>175271.78400000031</v>
+        <v>2298347.8590000044</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
@@ -8720,7 +8720,7 @@
         <v>53790227.082999997</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>7307437.6159999985</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>23042336.320999995</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
@@ -8816,7 +8816,7 @@
         <v>7738255.3251869353</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>13</v>
       </c>
@@ -8861,995 +8861,995 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="29"/>
+      <c r="B1" s="28">
         <v>2014</v>
       </c>
-      <c r="C1" s="24">
+      <c r="C1" s="28">
         <v>2015</v>
       </c>
-      <c r="D1" s="24">
+      <c r="D1" s="28">
         <v>2016</v>
       </c>
-      <c r="E1" s="24">
+      <c r="E1" s="28">
         <v>2017</v>
       </c>
-      <c r="F1" s="24">
+      <c r="F1" s="28">
         <v>2018</v>
       </c>
-      <c r="G1" s="24">
+      <c r="G1" s="28">
         <v>2019</v>
       </c>
-      <c r="H1" s="24">
+      <c r="H1" s="28">
         <v>2020</v>
       </c>
-      <c r="I1" s="24">
+      <c r="I1" s="28">
         <v>2021</v>
       </c>
-      <c r="J1" s="24">
+      <c r="J1" s="28">
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="25"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="26"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
     </row>
-    <row r="4" spans="1:10" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="20">
         <f>SUM(B5:B12)</f>
         <v>41526.830519999996</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="20">
         <f t="shared" ref="C4:J4" si="0">SUM(C5:C12)</f>
         <v>41394.85727</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="20">
         <f t="shared" si="0"/>
         <v>41656.134439999994</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="20">
         <f t="shared" si="0"/>
         <v>42202.377619999999</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="20">
         <f t="shared" si="0"/>
         <v>42226.42164</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="20">
         <f t="shared" si="0"/>
         <v>41620.061159999997</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="20">
         <f t="shared" si="0"/>
         <v>40337.964950000001</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="20">
         <f t="shared" si="0"/>
         <v>39328.085370000001</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="20">
         <f t="shared" si="0"/>
         <v>39172.853230000001</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="22">
         <f>SUM('[1]1'!B5,'[1]2'!B5,'[1]3'!B5,'[1]4'!B5,'[1]5'!B5,'[1]6'!B5,'[1]7'!B5,'[1]8'!B5,'[1]9'!B5,'[1]10'!B5,'[1]11'!B5,'[1]12'!B5,'[1]13'!B5,'[1]14'!B5)</f>
         <v>0</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="22">
         <f>SUM('[1]1'!C5,'[1]2'!C5,'[1]3'!C5,'[1]4'!C5,'[1]5'!C5,'[1]6'!C5,'[1]7'!C5,'[1]8'!C5,'[1]9'!C5,'[1]10'!C5,'[1]11'!C5,'[1]12'!C5,'[1]13'!C5,'[1]14'!C5)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="22">
         <f>SUM('[1]1'!D5,'[1]2'!D5,'[1]3'!D5,'[1]4'!D5,'[1]5'!D5,'[1]6'!D5,'[1]7'!D5,'[1]8'!D5,'[1]9'!D5,'[1]10'!D5,'[1]11'!D5,'[1]12'!D5,'[1]13'!D5,'[1]14'!D5)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="22">
         <f>SUM('[1]1'!E5,'[1]2'!E5,'[1]3'!E5,'[1]4'!E5,'[1]5'!E5,'[1]6'!E5,'[1]7'!E5,'[1]8'!E5,'[1]9'!E5,'[1]10'!E5,'[1]11'!E5,'[1]12'!E5,'[1]13'!E5,'[1]14'!E5)</f>
         <v>0</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="22">
         <f>SUM('[1]1'!F5,'[1]2'!F5,'[1]3'!F5,'[1]4'!F5,'[1]5'!F5,'[1]6'!F5,'[1]7'!F5,'[1]8'!F5,'[1]9'!F5,'[1]10'!F5,'[1]11'!F5,'[1]12'!F5,'[1]13'!F5,'[1]14'!F5)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="22">
         <f>SUM('[1]1'!G5,'[1]2'!G5,'[1]3'!G5,'[1]4'!G5,'[1]5'!G5,'[1]6'!G5,'[1]7'!G5,'[1]8'!G5,'[1]9'!G5,'[1]10'!G5,'[1]11'!G5,'[1]12'!G5,'[1]13'!G5,'[1]14'!G5)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="22">
         <f>SUM('[1]1'!H5,'[1]2'!H5,'[1]3'!H5,'[1]4'!H5,'[1]5'!H5,'[1]6'!H5,'[1]7'!H5,'[1]8'!H5,'[1]9'!H5,'[1]10'!H5,'[1]11'!H5,'[1]12'!H5,'[1]13'!H5,'[1]14'!H5)</f>
         <v>0</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="22">
         <f>SUM('[1]1'!I5,'[1]2'!I5,'[1]3'!I5,'[1]4'!I5,'[1]5'!I5,'[1]6'!I5,'[1]7'!I5,'[1]8'!I5,'[1]9'!I5,'[1]10'!I5,'[1]11'!I5,'[1]12'!I5,'[1]13'!I5,'[1]14'!I5)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="22">
         <f>SUM('[1]1'!J5,'[1]2'!J5,'[1]3'!J5,'[1]4'!J5,'[1]5'!J5,'[1]6'!J5,'[1]7'!J5,'[1]8'!J5,'[1]9'!J5,'[1]10'!J5,'[1]11'!J5,'[1]12'!J5,'[1]13'!J5,'[1]14'!J5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="24">
         <f>SUM('[1]1'!B6,'[1]2'!B6,'[1]3'!B6,'[1]4'!B6,'[1]5'!B6,'[1]6'!B6,'[1]7'!B6,'[1]8'!B6,'[1]9'!B6,'[1]10'!B6,'[1]11'!B6,'[1]12'!B6,'[1]13'!B6,'[1]14'!B6)</f>
         <v>21940.907919999994</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="24">
         <f>SUM('[1]1'!C6,'[1]2'!C6,'[1]3'!C6,'[1]4'!C6,'[1]5'!C6,'[1]6'!C6,'[1]7'!C6,'[1]8'!C6,'[1]9'!C6,'[1]10'!C6,'[1]11'!C6,'[1]12'!C6,'[1]13'!C6,'[1]14'!C6)</f>
         <v>21877.646769999999</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="24">
         <f>SUM('[1]1'!D6,'[1]2'!D6,'[1]3'!D6,'[1]4'!D6,'[1]5'!D6,'[1]6'!D6,'[1]7'!D6,'[1]8'!D6,'[1]9'!D6,'[1]10'!D6,'[1]11'!D6,'[1]12'!D6,'[1]13'!D6,'[1]14'!D6)</f>
         <v>22006.976839999996</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="24">
         <f>SUM('[1]1'!E6,'[1]2'!E6,'[1]3'!E6,'[1]4'!E6,'[1]5'!E6,'[1]6'!E6,'[1]7'!E6,'[1]8'!E6,'[1]9'!E6,'[1]10'!E6,'[1]11'!E6,'[1]12'!E6,'[1]13'!E6,'[1]14'!E6)</f>
         <v>22293.605519999994</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="24">
         <f>SUM('[1]1'!F6,'[1]2'!F6,'[1]3'!F6,'[1]4'!F6,'[1]5'!F6,'[1]6'!F6,'[1]7'!F6,'[1]8'!F6,'[1]9'!F6,'[1]10'!F6,'[1]11'!F6,'[1]12'!F6,'[1]13'!F6,'[1]14'!F6)</f>
         <v>22302.55024</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="24">
         <f>SUM('[1]1'!G6,'[1]2'!G6,'[1]3'!G6,'[1]4'!G6,'[1]5'!G6,'[1]6'!G6,'[1]7'!G6,'[1]8'!G6,'[1]9'!G6,'[1]10'!G6,'[1]11'!G6,'[1]12'!G6,'[1]13'!G6,'[1]14'!G6)</f>
         <v>22014.280070000001</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="24">
         <f>SUM('[1]1'!H6,'[1]2'!H6,'[1]3'!H6,'[1]4'!H6,'[1]5'!H6,'[1]6'!H6,'[1]7'!H6,'[1]8'!H6,'[1]9'!H6,'[1]10'!H6,'[1]11'!H6,'[1]12'!H6,'[1]13'!H6,'[1]14'!H6)</f>
         <v>21378.455119999995</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="24">
         <f>SUM('[1]1'!I6,'[1]2'!I6,'[1]3'!I6,'[1]4'!I6,'[1]5'!I6,'[1]6'!I6,'[1]7'!I6,'[1]8'!I6,'[1]9'!I6,'[1]10'!I6,'[1]11'!I6,'[1]12'!I6,'[1]13'!I6,'[1]14'!I6)</f>
         <v>20877.60744</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="24">
         <f>SUM('[1]1'!J6,'[1]2'!J6,'[1]3'!J6,'[1]4'!J6,'[1]5'!J6,'[1]6'!J6,'[1]7'!J6,'[1]8'!J6,'[1]9'!J6,'[1]10'!J6,'[1]11'!J6,'[1]12'!J6,'[1]13'!J6,'[1]14'!J6)</f>
         <v>20806.162549999997</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="24">
         <f>SUM('[1]1'!B7,'[1]2'!B7,'[1]3'!B7,'[1]4'!B7,'[1]5'!B7,'[1]6'!B7,'[1]7'!B7,'[1]8'!B7,'[1]9'!B7,'[1]10'!B7,'[1]11'!B7,'[1]12'!B7,'[1]13'!B7,'[1]14'!B7)</f>
         <v>4290</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="24">
         <f>SUM('[1]1'!C7,'[1]2'!C7,'[1]3'!C7,'[1]4'!C7,'[1]5'!C7,'[1]6'!C7,'[1]7'!C7,'[1]8'!C7,'[1]9'!C7,'[1]10'!C7,'[1]11'!C7,'[1]12'!C7,'[1]13'!C7,'[1]14'!C7)</f>
         <v>4290</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="24">
         <f>SUM('[1]1'!D7,'[1]2'!D7,'[1]3'!D7,'[1]4'!D7,'[1]5'!D7,'[1]6'!D7,'[1]7'!D7,'[1]8'!D7,'[1]9'!D7,'[1]10'!D7,'[1]11'!D7,'[1]12'!D7,'[1]13'!D7,'[1]14'!D7)</f>
         <v>4290</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="24">
         <f>SUM('[1]1'!E7,'[1]2'!E7,'[1]3'!E7,'[1]4'!E7,'[1]5'!E7,'[1]6'!E7,'[1]7'!E7,'[1]8'!E7,'[1]9'!E7,'[1]10'!E7,'[1]11'!E7,'[1]12'!E7,'[1]13'!E7,'[1]14'!E7)</f>
         <v>4290</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="24">
         <f>SUM('[1]1'!F7,'[1]2'!F7,'[1]3'!F7,'[1]4'!F7,'[1]5'!F7,'[1]6'!F7,'[1]7'!F7,'[1]8'!F7,'[1]9'!F7,'[1]10'!F7,'[1]11'!F7,'[1]12'!F7,'[1]13'!F7,'[1]14'!F7)</f>
         <v>4290</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="24">
         <f>SUM('[1]1'!G7,'[1]2'!G7,'[1]3'!G7,'[1]4'!G7,'[1]5'!G7,'[1]6'!G7,'[1]7'!G7,'[1]8'!G7,'[1]9'!G7,'[1]10'!G7,'[1]11'!G7,'[1]12'!G7,'[1]13'!G7,'[1]14'!G7)</f>
         <v>4290</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="24">
         <f>SUM('[1]1'!H7,'[1]2'!H7,'[1]3'!H7,'[1]4'!H7,'[1]5'!H7,'[1]6'!H7,'[1]7'!H7,'[1]8'!H7,'[1]9'!H7,'[1]10'!H7,'[1]11'!H7,'[1]12'!H7,'[1]13'!H7,'[1]14'!H7)</f>
         <v>4290</v>
       </c>
-      <c r="I7" s="32">
+      <c r="I7" s="24">
         <f>SUM('[1]1'!I7,'[1]2'!I7,'[1]3'!I7,'[1]4'!I7,'[1]5'!I7,'[1]6'!I7,'[1]7'!I7,'[1]8'!I7,'[1]9'!I7,'[1]10'!I7,'[1]11'!I7,'[1]12'!I7,'[1]13'!I7,'[1]14'!I7)</f>
         <v>4290</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="24">
         <f>SUM('[1]1'!J7,'[1]2'!J7,'[1]3'!J7,'[1]4'!J7,'[1]5'!J7,'[1]6'!J7,'[1]7'!J7,'[1]8'!J7,'[1]9'!J7,'[1]10'!J7,'[1]11'!J7,'[1]12'!J7,'[1]13'!J7,'[1]14'!J7)</f>
         <v>4290</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="31" t="s">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="24">
         <f>SUM('[1]1'!B8,'[1]2'!B8,'[1]3'!B8,'[1]4'!B8,'[1]5'!B8,'[1]6'!B8,'[1]7'!B8,'[1]8'!B8,'[1]9'!B8,'[1]10'!B8,'[1]11'!B8,'[1]12'!B8,'[1]13'!B8,'[1]14'!B8)</f>
         <v>10836.704400000001</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="24">
         <f>SUM('[1]1'!C8,'[1]2'!C8,'[1]3'!C8,'[1]4'!C8,'[1]5'!C8,'[1]6'!C8,'[1]7'!C8,'[1]8'!C8,'[1]9'!C8,'[1]10'!C8,'[1]11'!C8,'[1]12'!C8,'[1]13'!C8,'[1]14'!C8)</f>
         <v>10741.852000000001</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="24">
         <f>SUM('[1]1'!D8,'[1]2'!D8,'[1]3'!D8,'[1]4'!D8,'[1]5'!D8,'[1]6'!D8,'[1]7'!D8,'[1]8'!D8,'[1]9'!D8,'[1]10'!D8,'[1]11'!D8,'[1]12'!D8,'[1]13'!D8,'[1]14'!D8)</f>
         <v>10849.975000000002</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="24">
         <f>SUM('[1]1'!E8,'[1]2'!E8,'[1]3'!E8,'[1]4'!E8,'[1]5'!E8,'[1]6'!E8,'[1]7'!E8,'[1]8'!E8,'[1]9'!E8,'[1]10'!E8,'[1]11'!E8,'[1]12'!E8,'[1]13'!E8,'[1]14'!E8)</f>
         <v>11075.524000000001</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="24">
         <f>SUM('[1]1'!F8,'[1]2'!F8,'[1]3'!F8,'[1]4'!F8,'[1]5'!F8,'[1]6'!F8,'[1]7'!F8,'[1]8'!F8,'[1]9'!F8,'[1]10'!F8,'[1]11'!F8,'[1]12'!F8,'[1]13'!F8,'[1]14'!F8)</f>
         <v>11075.442000000001</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="24">
         <f>SUM('[1]1'!G8,'[1]2'!G8,'[1]3'!G8,'[1]4'!G8,'[1]5'!G8,'[1]6'!G8,'[1]7'!G8,'[1]8'!G8,'[1]9'!G8,'[1]10'!G8,'[1]11'!G8,'[1]12'!G8,'[1]13'!G8,'[1]14'!G8)</f>
         <v>10729.869000000001</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="24">
         <f>SUM('[1]1'!H8,'[1]2'!H8,'[1]3'!H8,'[1]4'!H8,'[1]5'!H8,'[1]6'!H8,'[1]7'!H8,'[1]8'!H8,'[1]9'!H8,'[1]10'!H8,'[1]11'!H8,'[1]12'!H8,'[1]13'!H8,'[1]14'!H8)</f>
         <v>10058.848</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="24">
         <f>SUM('[1]1'!I8,'[1]2'!I8,'[1]3'!I8,'[1]4'!I8,'[1]5'!I8,'[1]6'!I8,'[1]7'!I8,'[1]8'!I8,'[1]9'!I8,'[1]10'!I8,'[1]11'!I8,'[1]12'!I8,'[1]13'!I8,'[1]14'!I8)</f>
         <v>9527.6949999999997</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="24">
         <f>SUM('[1]1'!J8,'[1]2'!J8,'[1]3'!J8,'[1]4'!J8,'[1]5'!J8,'[1]6'!J8,'[1]7'!J8,'[1]8'!J8,'[1]9'!J8,'[1]10'!J8,'[1]11'!J8,'[1]12'!J8,'[1]13'!J8,'[1]14'!J8)</f>
         <v>9415.8970000000008</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="24">
         <f>SUM('[1]1'!B9,'[1]2'!B9,'[1]3'!B9,'[1]4'!B9,'[1]5'!B9,'[1]6'!B9,'[1]7'!B9,'[1]8'!B9,'[1]9'!B9,'[1]10'!B9,'[1]11'!B9,'[1]12'!B9,'[1]13'!B9,'[1]14'!B9)</f>
         <v>1363</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="24">
         <f>SUM('[1]1'!C9,'[1]2'!C9,'[1]3'!C9,'[1]4'!C9,'[1]5'!C9,'[1]6'!C9,'[1]7'!C9,'[1]8'!C9,'[1]9'!C9,'[1]10'!C9,'[1]11'!C9,'[1]12'!C9,'[1]13'!C9,'[1]14'!C9)</f>
         <v>1363.3150000000001</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="24">
         <f>SUM('[1]1'!D9,'[1]2'!D9,'[1]3'!D9,'[1]4'!D9,'[1]5'!D9,'[1]6'!D9,'[1]7'!D9,'[1]8'!D9,'[1]9'!D9,'[1]10'!D9,'[1]11'!D9,'[1]12'!D9,'[1]13'!D9,'[1]14'!D9)</f>
         <v>1363.5</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="24">
         <f>SUM('[1]1'!E9,'[1]2'!E9,'[1]3'!E9,'[1]4'!E9,'[1]5'!E9,'[1]6'!E9,'[1]7'!E9,'[1]8'!E9,'[1]9'!E9,'[1]10'!E9,'[1]11'!E9,'[1]12'!E9,'[1]13'!E9,'[1]14'!E9)</f>
         <v>1363.5</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="24">
         <f>SUM('[1]1'!F9,'[1]2'!F9,'[1]3'!F9,'[1]4'!F9,'[1]5'!F9,'[1]6'!F9,'[1]7'!F9,'[1]8'!F9,'[1]9'!F9,'[1]10'!F9,'[1]11'!F9,'[1]12'!F9,'[1]13'!F9,'[1]14'!F9)</f>
         <v>1363.5</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="24">
         <f>SUM('[1]1'!G9,'[1]2'!G9,'[1]3'!G9,'[1]4'!G9,'[1]5'!G9,'[1]6'!G9,'[1]7'!G9,'[1]8'!G9,'[1]9'!G9,'[1]10'!G9,'[1]11'!G9,'[1]12'!G9,'[1]13'!G9,'[1]14'!G9)</f>
         <v>1363.5</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="24">
         <f>SUM('[1]1'!H9,'[1]2'!H9,'[1]3'!H9,'[1]4'!H9,'[1]5'!H9,'[1]6'!H9,'[1]7'!H9,'[1]8'!H9,'[1]9'!H9,'[1]10'!H9,'[1]11'!H9,'[1]12'!H9,'[1]13'!H9,'[1]14'!H9)</f>
         <v>1363.5</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="24">
         <f>SUM('[1]1'!I9,'[1]2'!I9,'[1]3'!I9,'[1]4'!I9,'[1]5'!I9,'[1]6'!I9,'[1]7'!I9,'[1]8'!I9,'[1]9'!I9,'[1]10'!I9,'[1]11'!I9,'[1]12'!I9,'[1]13'!I9,'[1]14'!I9)</f>
         <v>1363.5</v>
       </c>
-      <c r="J9" s="32">
+      <c r="J9" s="24">
         <f>SUM('[1]1'!J9,'[1]2'!J9,'[1]3'!J9,'[1]4'!J9,'[1]5'!J9,'[1]6'!J9,'[1]7'!J9,'[1]8'!J9,'[1]9'!J9,'[1]10'!J9,'[1]11'!J9,'[1]12'!J9,'[1]13'!J9,'[1]14'!J9)</f>
         <v>1363.5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="31" t="s">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="24">
         <f>SUM('[1]1'!B10,'[1]2'!B10,'[1]3'!B10,'[1]4'!B10,'[1]5'!B10,'[1]6'!B10,'[1]7'!B10,'[1]8'!B10,'[1]9'!B10,'[1]10'!B10,'[1]11'!B10,'[1]12'!B10,'[1]13'!B10,'[1]14'!B10)</f>
         <v>833.66899999999998</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="24">
         <f>SUM('[1]1'!C10,'[1]2'!C10,'[1]3'!C10,'[1]4'!C10,'[1]5'!C10,'[1]6'!C10,'[1]7'!C10,'[1]8'!C10,'[1]9'!C10,'[1]10'!C10,'[1]11'!C10,'[1]12'!C10,'[1]13'!C10,'[1]14'!C10)</f>
         <v>855.5630000000001</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="24">
         <f>SUM('[1]1'!D10,'[1]2'!D10,'[1]3'!D10,'[1]4'!D10,'[1]5'!D10,'[1]6'!D10,'[1]7'!D10,'[1]8'!D10,'[1]9'!D10,'[1]10'!D10,'[1]11'!D10,'[1]12'!D10,'[1]13'!D10,'[1]14'!D10)</f>
         <v>873.99199999999996</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="24">
         <f>SUM('[1]1'!E10,'[1]2'!E10,'[1]3'!E10,'[1]4'!E10,'[1]5'!E10,'[1]6'!E10,'[1]7'!E10,'[1]8'!E10,'[1]9'!E10,'[1]10'!E10,'[1]11'!E10,'[1]12'!E10,'[1]13'!E10,'[1]14'!E10)</f>
         <v>895.98699999999985</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="24">
         <f>SUM('[1]1'!F10,'[1]2'!F10,'[1]3'!F10,'[1]4'!F10,'[1]5'!F10,'[1]6'!F10,'[1]7'!F10,'[1]8'!F10,'[1]9'!F10,'[1]10'!F10,'[1]11'!F10,'[1]12'!F10,'[1]13'!F10,'[1]14'!F10)</f>
         <v>910.90980000000002</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="24">
         <f>SUM('[1]1'!G10,'[1]2'!G10,'[1]3'!G10,'[1]4'!G10,'[1]5'!G10,'[1]6'!G10,'[1]7'!G10,'[1]8'!G10,'[1]9'!G10,'[1]10'!G10,'[1]11'!G10,'[1]12'!G10,'[1]13'!G10,'[1]14'!G10)</f>
         <v>937.70399999999995</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="24">
         <f>SUM('[1]1'!H10,'[1]2'!H10,'[1]3'!H10,'[1]4'!H10,'[1]5'!H10,'[1]6'!H10,'[1]7'!H10,'[1]8'!H10,'[1]9'!H10,'[1]10'!H10,'[1]11'!H10,'[1]12'!H10,'[1]13'!H10,'[1]14'!H10)</f>
         <v>961.74929999999995</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="24">
         <f>SUM('[1]1'!I10,'[1]2'!I10,'[1]3'!I10,'[1]4'!I10,'[1]5'!I10,'[1]6'!I10,'[1]7'!I10,'[1]8'!I10,'[1]9'!I10,'[1]10'!I10,'[1]11'!I10,'[1]12'!I10,'[1]13'!I10,'[1]14'!I10)</f>
         <v>983.15179999999987</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="24">
         <f>SUM('[1]1'!J10,'[1]2'!J10,'[1]3'!J10,'[1]4'!J10,'[1]5'!J10,'[1]6'!J10,'[1]7'!J10,'[1]8'!J10,'[1]9'!J10,'[1]10'!J10,'[1]11'!J10,'[1]12'!J10,'[1]13'!J10,'[1]14'!J10)</f>
         <v>1012.2180000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="31" t="s">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="24">
         <f>SUM('[1]1'!B11,'[1]2'!B11,'[1]3'!B11,'[1]4'!B11,'[1]5'!B11,'[1]6'!B11,'[1]7'!B11,'[1]8'!B11,'[1]9'!B11,'[1]10'!B11,'[1]11'!B11,'[1]12'!B11,'[1]13'!B11,'[1]14'!B11)</f>
         <v>1091.0491999999999</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="24">
         <f>SUM('[1]1'!C11,'[1]2'!C11,'[1]3'!C11,'[1]4'!C11,'[1]5'!C11,'[1]6'!C11,'[1]7'!C11,'[1]8'!C11,'[1]9'!C11,'[1]10'!C11,'[1]11'!C11,'[1]12'!C11,'[1]13'!C11,'[1]14'!C11)</f>
         <v>1094.9804999999999</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="24">
         <f>SUM('[1]1'!D11,'[1]2'!D11,'[1]3'!D11,'[1]4'!D11,'[1]5'!D11,'[1]6'!D11,'[1]7'!D11,'[1]8'!D11,'[1]9'!D11,'[1]10'!D11,'[1]11'!D11,'[1]12'!D11,'[1]13'!D11,'[1]14'!D11)</f>
         <v>1100.1906000000001</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="24">
         <f>SUM('[1]1'!E11,'[1]2'!E11,'[1]3'!E11,'[1]4'!E11,'[1]5'!E11,'[1]6'!E11,'[1]7'!E11,'[1]8'!E11,'[1]9'!E11,'[1]10'!E11,'[1]11'!E11,'[1]12'!E11,'[1]13'!E11,'[1]14'!E11)</f>
         <v>1112.2610999999999</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="24">
         <f>SUM('[1]1'!F11,'[1]2'!F11,'[1]3'!F11,'[1]4'!F11,'[1]5'!F11,'[1]6'!F11,'[1]7'!F11,'[1]8'!F11,'[1]9'!F11,'[1]10'!F11,'[1]11'!F11,'[1]12'!F11,'[1]13'!F11,'[1]14'!F11)</f>
         <v>1112.5196000000003</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="24">
         <f>SUM('[1]1'!G11,'[1]2'!G11,'[1]3'!G11,'[1]4'!G11,'[1]5'!G11,'[1]6'!G11,'[1]7'!G11,'[1]8'!G11,'[1]9'!G11,'[1]10'!G11,'[1]11'!G11,'[1]12'!G11,'[1]13'!G11,'[1]14'!G11)</f>
         <v>1113.2080900000001</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="24">
         <f>SUM('[1]1'!H11,'[1]2'!H11,'[1]3'!H11,'[1]4'!H11,'[1]5'!H11,'[1]6'!H11,'[1]7'!H11,'[1]8'!H11,'[1]9'!H11,'[1]10'!H11,'[1]11'!H11,'[1]12'!H11,'[1]13'!H11,'[1]14'!H11)</f>
         <v>1113.9125300000001</v>
       </c>
-      <c r="I11" s="32">
+      <c r="I11" s="24">
         <f>SUM('[1]1'!I11,'[1]2'!I11,'[1]3'!I11,'[1]4'!I11,'[1]5'!I11,'[1]6'!I11,'[1]7'!I11,'[1]8'!I11,'[1]9'!I11,'[1]10'!I11,'[1]11'!I11,'[1]12'!I11,'[1]13'!I11,'[1]14'!I11)</f>
         <v>1114.63113</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J11" s="24">
         <f>SUM('[1]1'!J11,'[1]2'!J11,'[1]3'!J11,'[1]4'!J11,'[1]5'!J11,'[1]6'!J11,'[1]7'!J11,'[1]8'!J11,'[1]9'!J11,'[1]10'!J11,'[1]11'!J11,'[1]12'!J11,'[1]13'!J11,'[1]14'!J11)</f>
         <v>1113.5756799999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="33" t="s">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="24">
         <f>SUM('[1]1'!B12,'[1]2'!B12,'[1]3'!B12,'[1]4'!B12,'[1]5'!B12,'[1]6'!B12,'[1]7'!B12,'[1]8'!B12,'[1]9'!B12,'[1]10'!B12,'[1]11'!B12,'[1]12'!B12,'[1]13'!B12,'[1]14'!B12)</f>
         <v>1171.5</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="24">
         <f>SUM('[1]1'!C12,'[1]2'!C12,'[1]3'!C12,'[1]4'!C12,'[1]5'!C12,'[1]6'!C12,'[1]7'!C12,'[1]8'!C12,'[1]9'!C12,'[1]10'!C12,'[1]11'!C12,'[1]12'!C12,'[1]13'!C12,'[1]14'!C12)</f>
         <v>1171.5</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="24">
         <f>SUM('[1]1'!D12,'[1]2'!D12,'[1]3'!D12,'[1]4'!D12,'[1]5'!D12,'[1]6'!D12,'[1]7'!D12,'[1]8'!D12,'[1]9'!D12,'[1]10'!D12,'[1]11'!D12,'[1]12'!D12,'[1]13'!D12,'[1]14'!D12)</f>
         <v>1171.5</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="24">
         <f>SUM('[1]1'!E12,'[1]2'!E12,'[1]3'!E12,'[1]4'!E12,'[1]5'!E12,'[1]6'!E12,'[1]7'!E12,'[1]8'!E12,'[1]9'!E12,'[1]10'!E12,'[1]11'!E12,'[1]12'!E12,'[1]13'!E12,'[1]14'!E12)</f>
         <v>1171.5</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="24">
         <f>SUM('[1]1'!F12,'[1]2'!F12,'[1]3'!F12,'[1]4'!F12,'[1]5'!F12,'[1]6'!F12,'[1]7'!F12,'[1]8'!F12,'[1]9'!F12,'[1]10'!F12,'[1]11'!F12,'[1]12'!F12,'[1]13'!F12,'[1]14'!F12)</f>
         <v>1171.5</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="24">
         <f>SUM('[1]1'!G12,'[1]2'!G12,'[1]3'!G12,'[1]4'!G12,'[1]5'!G12,'[1]6'!G12,'[1]7'!G12,'[1]8'!G12,'[1]9'!G12,'[1]10'!G12,'[1]11'!G12,'[1]12'!G12,'[1]13'!G12,'[1]14'!G12)</f>
         <v>1171.5</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="24">
         <f>SUM('[1]1'!H12,'[1]2'!H12,'[1]3'!H12,'[1]4'!H12,'[1]5'!H12,'[1]6'!H12,'[1]7'!H12,'[1]8'!H12,'[1]9'!H12,'[1]10'!H12,'[1]11'!H12,'[1]12'!H12,'[1]13'!H12,'[1]14'!H12)</f>
         <v>1171.5</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="24">
         <f>SUM('[1]1'!I12,'[1]2'!I12,'[1]3'!I12,'[1]4'!I12,'[1]5'!I12,'[1]6'!I12,'[1]7'!I12,'[1]8'!I12,'[1]9'!I12,'[1]10'!I12,'[1]11'!I12,'[1]12'!I12,'[1]13'!I12,'[1]14'!I12)</f>
         <v>1171.5</v>
       </c>
-      <c r="J12" s="32">
+      <c r="J12" s="24">
         <f>SUM('[1]1'!J12,'[1]2'!J12,'[1]3'!J12,'[1]4'!J12,'[1]5'!J12,'[1]6'!J12,'[1]7'!J12,'[1]8'!J12,'[1]9'!J12,'[1]10'!J12,'[1]11'!J12,'[1]12'!J12,'[1]13'!J12,'[1]14'!J12)</f>
         <v>1171.5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="27" t="s">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="20">
         <f>SUM(B14:B21)</f>
         <v>168548927.22962007</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="20">
         <f t="shared" ref="C13:J13" si="1">SUM(C14:C21)</f>
         <v>163849009.58366999</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="20">
         <f t="shared" si="1"/>
         <v>162955887.10934007</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="20">
         <f t="shared" si="1"/>
         <v>170301522.83002001</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="20">
         <f t="shared" si="1"/>
         <v>172180583.21744001</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="20">
         <f t="shared" si="1"/>
         <v>170005369.50658002</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="20">
         <f t="shared" si="1"/>
         <v>158839720.47188997</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="20">
         <f t="shared" si="1"/>
         <v>166028084.29711002</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="20">
         <f t="shared" si="1"/>
         <v>165254240.03297001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="29" t="s">
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="22">
         <f>SUM('[1]1'!B14,'[1]2'!B14,'[1]3'!B14,'[1]4'!B14,'[1]5'!B14,'[1]6'!B14,'[1]7'!B14,'[1]8'!B14,'[1]9'!B14,'[1]10'!B14,'[1]11'!B14,'[1]12'!B14,'[1]13'!B14,'[1]14'!B14)</f>
         <v>2076.7944199999956</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="22">
         <f>SUM('[1]1'!C14,'[1]2'!C14,'[1]3'!C14,'[1]4'!C14,'[1]5'!C14,'[1]6'!C14,'[1]7'!C14,'[1]8'!C14,'[1]9'!C14,'[1]10'!C14,'[1]11'!C14,'[1]12'!C14,'[1]13'!C14,'[1]14'!C14)</f>
         <v>2078.2503699999952</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="22">
         <f>SUM('[1]1'!D14,'[1]2'!D14,'[1]3'!D14,'[1]4'!D14,'[1]5'!D14,'[1]6'!D14,'[1]7'!D14,'[1]8'!D14,'[1]9'!D14,'[1]10'!D14,'[1]11'!D14,'[1]12'!D14,'[1]13'!D14,'[1]14'!D14)</f>
         <v>2075.6643399999962</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="22">
         <f>SUM('[1]1'!E14,'[1]2'!E14,'[1]3'!E14,'[1]4'!E14,'[1]5'!E14,'[1]6'!E14,'[1]7'!E14,'[1]8'!E14,'[1]9'!E14,'[1]10'!E14,'[1]11'!E14,'[1]12'!E14,'[1]13'!E14,'[1]14'!E14)</f>
         <v>2076.6260199999956</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="22">
         <f>SUM('[1]1'!F14,'[1]2'!F14,'[1]3'!F14,'[1]4'!F14,'[1]5'!F14,'[1]6'!F14,'[1]7'!F14,'[1]8'!F14,'[1]9'!F14,'[1]10'!F14,'[1]11'!F14,'[1]12'!F14,'[1]13'!F14,'[1]14'!F14)</f>
         <v>2061.9714399999957</v>
       </c>
-      <c r="G14" s="30">
+      <c r="G14" s="22">
         <f>SUM('[1]1'!G14,'[1]2'!G14,'[1]3'!G14,'[1]4'!G14,'[1]5'!G14,'[1]6'!G14,'[1]7'!G14,'[1]8'!G14,'[1]9'!G14,'[1]10'!G14,'[1]11'!G14,'[1]12'!G14,'[1]13'!G14,'[1]14'!G14)</f>
         <v>2069.0745799999959</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="22">
         <f>SUM('[1]1'!H14,'[1]2'!H14,'[1]3'!H14,'[1]4'!H14,'[1]5'!H14,'[1]6'!H14,'[1]7'!H14,'[1]8'!H14,'[1]9'!H14,'[1]10'!H14,'[1]11'!H14,'[1]12'!H14,'[1]13'!H14,'[1]14'!H14)</f>
         <v>2079.5208899999966</v>
       </c>
-      <c r="I14" s="30">
+      <c r="I14" s="22">
         <f>SUM('[1]1'!I14,'[1]2'!I14,'[1]3'!I14,'[1]4'!I14,'[1]5'!I14,'[1]6'!I14,'[1]7'!I14,'[1]8'!I14,'[1]9'!I14,'[1]10'!I14,'[1]11'!I14,'[1]12'!I14,'[1]13'!I14,'[1]14'!I14)</f>
         <v>2087.7051099999958</v>
       </c>
-      <c r="J14" s="30">
+      <c r="J14" s="22">
         <f>SUM('[1]1'!J14,'[1]2'!J14,'[1]3'!J14,'[1]4'!J14,'[1]5'!J14,'[1]6'!J14,'[1]7'!J14,'[1]8'!J14,'[1]9'!J14,'[1]10'!J14,'[1]11'!J14,'[1]12'!J14,'[1]13'!J14,'[1]14'!J14)</f>
         <v>2100.3769699999957</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="31" t="s">
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="24">
         <f>SUM('[1]1'!B15,'[1]2'!B15,'[1]3'!B15,'[1]4'!B15,'[1]5'!B15,'[1]6'!B15,'[1]7'!B15,'[1]8'!B15,'[1]9'!B15,'[1]10'!B15,'[1]11'!B15,'[1]12'!B15,'[1]13'!B15,'[1]14'!B15)</f>
         <v>86013493.427200034</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="24">
         <f>SUM('[1]1'!C15,'[1]2'!C15,'[1]3'!C15,'[1]4'!C15,'[1]5'!C15,'[1]6'!C15,'[1]7'!C15,'[1]8'!C15,'[1]9'!C15,'[1]10'!C15,'[1]11'!C15,'[1]12'!C15,'[1]13'!C15,'[1]14'!C15)</f>
         <v>83893758.431299984</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="24">
         <f>SUM('[1]1'!D15,'[1]2'!D15,'[1]3'!D15,'[1]4'!D15,'[1]5'!D15,'[1]6'!D15,'[1]7'!D15,'[1]8'!D15,'[1]9'!D15,'[1]10'!D15,'[1]11'!D15,'[1]12'!D15,'[1]13'!D15,'[1]14'!D15)</f>
         <v>83305632.317000017</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="24">
         <f>SUM('[1]1'!E15,'[1]2'!E15,'[1]3'!E15,'[1]4'!E15,'[1]5'!E15,'[1]6'!E15,'[1]7'!E15,'[1]8'!E15,'[1]9'!E15,'[1]10'!E15,'[1]11'!E15,'[1]12'!E15,'[1]13'!E15,'[1]14'!E15)</f>
         <v>87041288.026999995</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="24">
         <f>SUM('[1]1'!F15,'[1]2'!F15,'[1]3'!F15,'[1]4'!F15,'[1]5'!F15,'[1]6'!F15,'[1]7'!F15,'[1]8'!F15,'[1]9'!F15,'[1]10'!F15,'[1]11'!F15,'[1]12'!F15,'[1]13'!F15,'[1]14'!F15)</f>
         <v>88002380.354999989</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="24">
         <f>SUM('[1]1'!G15,'[1]2'!G15,'[1]3'!G15,'[1]4'!G15,'[1]5'!G15,'[1]6'!G15,'[1]7'!G15,'[1]8'!G15,'[1]9'!G15,'[1]10'!G15,'[1]11'!G15,'[1]12'!G15,'[1]13'!G15,'[1]14'!G15)</f>
         <v>86991236.566000015</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="24">
         <f>SUM('[1]1'!H15,'[1]2'!H15,'[1]3'!H15,'[1]4'!H15,'[1]5'!H15,'[1]6'!H15,'[1]7'!H15,'[1]8'!H15,'[1]9'!H15,'[1]10'!H15,'[1]11'!H15,'[1]12'!H15,'[1]13'!H15,'[1]14'!H15)</f>
         <v>81445899.992999986</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="24">
         <f>SUM('[1]1'!I15,'[1]2'!I15,'[1]3'!I15,'[1]4'!I15,'[1]5'!I15,'[1]6'!I15,'[1]7'!I15,'[1]8'!I15,'[1]9'!I15,'[1]10'!I15,'[1]11'!I15,'[1]12'!I15,'[1]13'!I15,'[1]14'!I15)</f>
         <v>84907950.802000001</v>
       </c>
-      <c r="J15" s="32">
+      <c r="J15" s="24">
         <f>SUM('[1]1'!J15,'[1]2'!J15,'[1]3'!J15,'[1]4'!J15,'[1]5'!J15,'[1]6'!J15,'[1]7'!J15,'[1]8'!J15,'[1]9'!J15,'[1]10'!J15,'[1]11'!J15,'[1]12'!J15,'[1]13'!J15,'[1]14'!J15)</f>
         <v>84503127.281000003</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="31" t="s">
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="24">
         <f>SUM('[1]1'!B16,'[1]2'!B16,'[1]3'!B16,'[1]4'!B16,'[1]5'!B16,'[1]6'!B16,'[1]7'!B16,'[1]8'!B16,'[1]9'!B16,'[1]10'!B16,'[1]11'!B16,'[1]12'!B16,'[1]13'!B16,'[1]14'!B16)</f>
         <v>30324873.359999999</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="24">
         <f>SUM('[1]1'!C16,'[1]2'!C16,'[1]3'!C16,'[1]4'!C16,'[1]5'!C16,'[1]6'!C16,'[1]7'!C16,'[1]8'!C16,'[1]9'!C16,'[1]10'!C16,'[1]11'!C16,'[1]12'!C16,'[1]13'!C16,'[1]14'!C16)</f>
         <v>26840847.649999999</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="24">
         <f>SUM('[1]1'!D16,'[1]2'!D16,'[1]3'!D16,'[1]4'!D16,'[1]5'!D16,'[1]6'!D16,'[1]7'!D16,'[1]8'!D16,'[1]9'!D16,'[1]10'!D16,'[1]11'!D16,'[1]12'!D16,'[1]13'!D16,'[1]14'!D16)</f>
         <v>24104222.150000002</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="24">
         <f>SUM('[1]1'!E16,'[1]2'!E16,'[1]3'!E16,'[1]4'!E16,'[1]5'!E16,'[1]6'!E16,'[1]7'!E16,'[1]8'!E16,'[1]9'!E16,'[1]10'!E16,'[1]11'!E16,'[1]12'!E16,'[1]13'!E16,'[1]14'!E16)</f>
         <v>28339577.039999999</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="24">
         <f>SUM('[1]1'!F16,'[1]2'!F16,'[1]3'!F16,'[1]4'!F16,'[1]5'!F16,'[1]6'!F16,'[1]7'!F16,'[1]8'!F16,'[1]9'!F16,'[1]10'!F16,'[1]11'!F16,'[1]12'!F16,'[1]13'!F16,'[1]14'!F16)</f>
         <v>29921311.170000002</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="24">
         <f>SUM('[1]1'!G16,'[1]2'!G16,'[1]3'!G16,'[1]4'!G16,'[1]5'!G16,'[1]6'!G16,'[1]7'!G16,'[1]8'!G16,'[1]9'!G16,'[1]10'!G16,'[1]11'!G16,'[1]12'!G16,'[1]13'!G16,'[1]14'!G16)</f>
         <v>30246208.84</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="24">
         <f>SUM('[1]1'!H16,'[1]2'!H16,'[1]3'!H16,'[1]4'!H16,'[1]5'!H16,'[1]6'!H16,'[1]7'!H16,'[1]8'!H16,'[1]9'!H16,'[1]10'!H16,'[1]11'!H16,'[1]12'!H16,'[1]13'!H16,'[1]14'!H16)</f>
         <v>30043279.77</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="24">
         <f>SUM('[1]1'!I16,'[1]2'!I16,'[1]3'!I16,'[1]4'!I16,'[1]5'!I16,'[1]6'!I16,'[1]7'!I16,'[1]8'!I16,'[1]9'!I16,'[1]10'!I16,'[1]11'!I16,'[1]12'!I16,'[1]13'!I16,'[1]14'!I16)</f>
         <v>30731180.379999999</v>
       </c>
-      <c r="J16" s="32">
+      <c r="J16" s="24">
         <f>SUM('[1]1'!J16,'[1]2'!J16,'[1]3'!J16,'[1]4'!J16,'[1]5'!J16,'[1]6'!J16,'[1]7'!J16,'[1]8'!J16,'[1]9'!J16,'[1]10'!J16,'[1]11'!J16,'[1]12'!J16,'[1]13'!J16,'[1]14'!J16)</f>
         <v>31021810.439999998</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="31" t="s">
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="24">
         <f>SUM('[1]1'!B17,'[1]2'!B17,'[1]3'!B17,'[1]4'!B17,'[1]5'!B17,'[1]6'!B17,'[1]7'!B17,'[1]8'!B17,'[1]9'!B17,'[1]10'!B17,'[1]11'!B17,'[1]12'!B17,'[1]13'!B17,'[1]14'!B17)</f>
         <v>44420480.449000016</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="24">
         <f>SUM('[1]1'!C17,'[1]2'!C17,'[1]3'!C17,'[1]4'!C17,'[1]5'!C17,'[1]6'!C17,'[1]7'!C17,'[1]8'!C17,'[1]9'!C17,'[1]10'!C17,'[1]11'!C17,'[1]12'!C17,'[1]13'!C17,'[1]14'!C17)</f>
         <v>44819831.069999985</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="24">
         <f>SUM('[1]1'!D17,'[1]2'!D17,'[1]3'!D17,'[1]4'!D17,'[1]5'!D17,'[1]6'!D17,'[1]7'!D17,'[1]8'!D17,'[1]9'!D17,'[1]10'!D17,'[1]11'!D17,'[1]12'!D17,'[1]13'!D17,'[1]14'!D17)</f>
         <v>45704070.480000004</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="24">
         <f>SUM('[1]1'!E17,'[1]2'!E17,'[1]3'!E17,'[1]4'!E17,'[1]5'!E17,'[1]6'!E17,'[1]7'!E17,'[1]8'!E17,'[1]9'!E17,'[1]10'!E17,'[1]11'!E17,'[1]12'!E17,'[1]13'!E17,'[1]14'!E17)</f>
         <v>45431680.267999992</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="24">
         <f>SUM('[1]1'!F17,'[1]2'!F17,'[1]3'!F17,'[1]4'!F17,'[1]5'!F17,'[1]6'!F17,'[1]7'!F17,'[1]8'!F17,'[1]9'!F17,'[1]10'!F17,'[1]11'!F17,'[1]12'!F17,'[1]13'!F17,'[1]14'!F17)</f>
         <v>45070754.584000006</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="24">
         <f>SUM('[1]1'!G17,'[1]2'!G17,'[1]3'!G17,'[1]4'!G17,'[1]5'!G17,'[1]6'!G17,'[1]7'!G17,'[1]8'!G17,'[1]9'!G17,'[1]10'!G17,'[1]11'!G17,'[1]12'!G17,'[1]13'!G17,'[1]14'!G17)</f>
         <v>41386690.89199999</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="24">
         <f>SUM('[1]1'!H17,'[1]2'!H17,'[1]3'!H17,'[1]4'!H17,'[1]5'!H17,'[1]6'!H17,'[1]7'!H17,'[1]8'!H17,'[1]9'!H17,'[1]10'!H17,'[1]11'!H17,'[1]12'!H17,'[1]13'!H17,'[1]14'!H17)</f>
         <v>35198100.92899999</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="24">
         <f>SUM('[1]1'!I17,'[1]2'!I17,'[1]3'!I17,'[1]4'!I17,'[1]5'!I17,'[1]6'!I17,'[1]7'!I17,'[1]8'!I17,'[1]9'!I17,'[1]10'!I17,'[1]11'!I17,'[1]12'!I17,'[1]13'!I17,'[1]14'!I17)</f>
         <v>38631451.995999992</v>
       </c>
-      <c r="J17" s="32">
+      <c r="J17" s="24">
         <f>SUM('[1]1'!J17,'[1]2'!J17,'[1]3'!J17,'[1]4'!J17,'[1]5'!J17,'[1]6'!J17,'[1]7'!J17,'[1]8'!J17,'[1]9'!J17,'[1]10'!J17,'[1]11'!J17,'[1]12'!J17,'[1]13'!J17,'[1]14'!J17)</f>
         <v>41017314.489</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="31" t="s">
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="24">
         <f>SUM('[1]1'!B18,'[1]2'!B18,'[1]3'!B18,'[1]4'!B18,'[1]5'!B18,'[1]6'!B18,'[1]7'!B18,'[1]8'!B18,'[1]9'!B18,'[1]10'!B18,'[1]11'!B18,'[1]12'!B18,'[1]13'!B18,'[1]14'!B18)</f>
         <v>2204674.9</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="24">
         <f>SUM('[1]1'!C18,'[1]2'!C18,'[1]3'!C18,'[1]4'!C18,'[1]5'!C18,'[1]6'!C18,'[1]7'!C18,'[1]8'!C18,'[1]9'!C18,'[1]10'!C18,'[1]11'!C18,'[1]12'!C18,'[1]13'!C18,'[1]14'!C18)</f>
         <v>2749023.0999999996</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="24">
         <f>SUM('[1]1'!D18,'[1]2'!D18,'[1]3'!D18,'[1]4'!D18,'[1]5'!D18,'[1]6'!D18,'[1]7'!D18,'[1]8'!D18,'[1]9'!D18,'[1]10'!D18,'[1]11'!D18,'[1]12'!D18,'[1]13'!D18,'[1]14'!D18)</f>
         <v>4049243.6780000003</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="24">
         <f>SUM('[1]1'!E18,'[1]2'!E18,'[1]3'!E18,'[1]4'!E18,'[1]5'!E18,'[1]6'!E18,'[1]7'!E18,'[1]8'!E18,'[1]9'!E18,'[1]10'!E18,'[1]11'!E18,'[1]12'!E18,'[1]13'!E18,'[1]14'!E18)</f>
         <v>3722405.4339999999</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="24">
         <f>SUM('[1]1'!F18,'[1]2'!F18,'[1]3'!F18,'[1]4'!F18,'[1]5'!F18,'[1]6'!F18,'[1]7'!F18,'[1]8'!F18,'[1]9'!F18,'[1]10'!F18,'[1]11'!F18,'[1]12'!F18,'[1]13'!F18,'[1]14'!F18)</f>
         <v>3690871.87</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="24">
         <f>SUM('[1]1'!G18,'[1]2'!G18,'[1]3'!G18,'[1]4'!G18,'[1]5'!G18,'[1]6'!G18,'[1]7'!G18,'[1]8'!G18,'[1]9'!G18,'[1]10'!G18,'[1]11'!G18,'[1]12'!G18,'[1]13'!G18,'[1]14'!G18)</f>
         <v>5518520.6710000001</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="24">
         <f>SUM('[1]1'!H18,'[1]2'!H18,'[1]3'!H18,'[1]4'!H18,'[1]5'!H18,'[1]6'!H18,'[1]7'!H18,'[1]8'!H18,'[1]9'!H18,'[1]10'!H18,'[1]11'!H18,'[1]12'!H18,'[1]13'!H18,'[1]14'!H18)</f>
         <v>6041267.5499999989</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I18" s="24">
         <f>SUM('[1]1'!I18,'[1]2'!I18,'[1]3'!I18,'[1]4'!I18,'[1]5'!I18,'[1]6'!I18,'[1]7'!I18,'[1]8'!I18,'[1]9'!I18,'[1]10'!I18,'[1]11'!I18,'[1]12'!I18,'[1]13'!I18,'[1]14'!I18)</f>
         <v>5239842.1099999994</v>
       </c>
-      <c r="J18" s="32">
+      <c r="J18" s="24">
         <f>SUM('[1]1'!J18,'[1]2'!J18,'[1]3'!J18,'[1]4'!J18,'[1]5'!J18,'[1]6'!J18,'[1]7'!J18,'[1]8'!J18,'[1]9'!J18,'[1]10'!J18,'[1]11'!J18,'[1]12'!J18,'[1]13'!J18,'[1]14'!J18)</f>
         <v>2533599.0180000002</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="31" t="s">
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="24">
         <f>SUM('[1]1'!B19,'[1]2'!B19,'[1]3'!B19,'[1]4'!B19,'[1]5'!B19,'[1]6'!B19,'[1]7'!B19,'[1]8'!B19,'[1]9'!B19,'[1]10'!B19,'[1]11'!B19,'[1]12'!B19,'[1]13'!B19,'[1]14'!B19)</f>
         <v>3498294.1009999998</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="24">
         <f>SUM('[1]1'!C19,'[1]2'!C19,'[1]3'!C19,'[1]4'!C19,'[1]5'!C19,'[1]6'!C19,'[1]7'!C19,'[1]8'!C19,'[1]9'!C19,'[1]10'!C19,'[1]11'!C19,'[1]12'!C19,'[1]13'!C19,'[1]14'!C19)</f>
         <v>3572812.2869999981</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="24">
         <f>SUM('[1]1'!D19,'[1]2'!D19,'[1]3'!D19,'[1]4'!D19,'[1]5'!D19,'[1]6'!D19,'[1]7'!D19,'[1]8'!D19,'[1]9'!D19,'[1]10'!D19,'[1]11'!D19,'[1]12'!D19,'[1]13'!D19,'[1]14'!D19)</f>
         <v>3613882.0269999984</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="24">
         <f>SUM('[1]1'!E19,'[1]2'!E19,'[1]3'!E19,'[1]4'!E19,'[1]5'!E19,'[1]6'!E19,'[1]7'!E19,'[1]8'!E19,'[1]9'!E19,'[1]10'!E19,'[1]11'!E19,'[1]12'!E19,'[1]13'!E19,'[1]14'!E19)</f>
         <v>3719689.5779999997</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="24">
         <f>SUM('[1]1'!F19,'[1]2'!F19,'[1]3'!F19,'[1]4'!F19,'[1]5'!F19,'[1]6'!F19,'[1]7'!F19,'[1]8'!F19,'[1]9'!F19,'[1]10'!F19,'[1]11'!F19,'[1]12'!F19,'[1]13'!F19,'[1]14'!F19)</f>
         <v>3690413.1099999994</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="24">
         <f>SUM('[1]1'!G19,'[1]2'!G19,'[1]3'!G19,'[1]4'!G19,'[1]5'!G19,'[1]6'!G19,'[1]7'!G19,'[1]8'!G19,'[1]9'!G19,'[1]10'!G19,'[1]11'!G19,'[1]12'!G19,'[1]13'!G19,'[1]14'!G19)</f>
         <v>3676697.149999999</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="24">
         <f>SUM('[1]1'!H19,'[1]2'!H19,'[1]3'!H19,'[1]4'!H19,'[1]5'!H19,'[1]6'!H19,'[1]7'!H19,'[1]8'!H19,'[1]9'!H19,'[1]10'!H19,'[1]11'!H19,'[1]12'!H19,'[1]13'!H19,'[1]14'!H19)</f>
         <v>3789565.7849999978</v>
       </c>
-      <c r="I19" s="32">
+      <c r="I19" s="24">
         <f>SUM('[1]1'!I19,'[1]2'!I19,'[1]3'!I19,'[1]4'!I19,'[1]5'!I19,'[1]6'!I19,'[1]7'!I19,'[1]8'!I19,'[1]9'!I19,'[1]10'!I19,'[1]11'!I19,'[1]12'!I19,'[1]13'!I19,'[1]14'!I19)</f>
         <v>3930065.0409999988</v>
       </c>
-      <c r="J19" s="32">
+      <c r="J19" s="24">
         <f>SUM('[1]1'!J19,'[1]2'!J19,'[1]3'!J19,'[1]4'!J19,'[1]5'!J19,'[1]6'!J19,'[1]7'!J19,'[1]8'!J19,'[1]9'!J19,'[1]10'!J19,'[1]11'!J19,'[1]12'!J19,'[1]13'!J19,'[1]14'!J19)</f>
         <v>3907551.2609999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="31" t="s">
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="24">
         <f>SUM('[1]1'!B20,'[1]2'!B20,'[1]3'!B20,'[1]4'!B20,'[1]5'!B20,'[1]6'!B20,'[1]7'!B20,'[1]8'!B20,'[1]9'!B20,'[1]10'!B20,'[1]11'!B20,'[1]12'!B20,'[1]13'!B20,'[1]14'!B20)</f>
         <v>1909762.4139999999</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="24">
         <f>SUM('[1]1'!C20,'[1]2'!C20,'[1]3'!C20,'[1]4'!C20,'[1]5'!C20,'[1]6'!C20,'[1]7'!C20,'[1]8'!C20,'[1]9'!C20,'[1]10'!C20,'[1]11'!C20,'[1]12'!C20,'[1]13'!C20,'[1]14'!C20)</f>
         <v>1795387.0110000004</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="24">
         <f>SUM('[1]1'!D20,'[1]2'!D20,'[1]3'!D20,'[1]4'!D20,'[1]5'!D20,'[1]6'!D20,'[1]7'!D20,'[1]8'!D20,'[1]9'!D20,'[1]10'!D20,'[1]11'!D20,'[1]12'!D20,'[1]13'!D20,'[1]14'!D20)</f>
         <v>2001489.0090000003</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="24">
         <f>SUM('[1]1'!E20,'[1]2'!E20,'[1]3'!E20,'[1]4'!E20,'[1]5'!E20,'[1]6'!E20,'[1]7'!E20,'[1]8'!E20,'[1]9'!E20,'[1]10'!E20,'[1]11'!E20,'[1]12'!E20,'[1]13'!E20,'[1]14'!E20)</f>
         <v>1869534.0729999996</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="24">
         <f>SUM('[1]1'!F20,'[1]2'!F20,'[1]3'!F20,'[1]4'!F20,'[1]5'!F20,'[1]6'!F20,'[1]7'!F20,'[1]8'!F20,'[1]9'!F20,'[1]10'!F20,'[1]11'!F20,'[1]12'!F20,'[1]13'!F20,'[1]14'!F20)</f>
         <v>1627518.3729999997</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="24">
         <f>SUM('[1]1'!G20,'[1]2'!G20,'[1]3'!G20,'[1]4'!G20,'[1]5'!G20,'[1]6'!G20,'[1]7'!G20,'[1]8'!G20,'[1]9'!G20,'[1]10'!G20,'[1]11'!G20,'[1]12'!G20,'[1]13'!G20,'[1]14'!G20)</f>
         <v>2008674.5289999996</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="24">
         <f>SUM('[1]1'!H20,'[1]2'!H20,'[1]3'!H20,'[1]4'!H20,'[1]5'!H20,'[1]6'!H20,'[1]7'!H20,'[1]8'!H20,'[1]9'!H20,'[1]10'!H20,'[1]11'!H20,'[1]12'!H20,'[1]13'!H20,'[1]14'!H20)</f>
         <v>2144255.1399999997</v>
       </c>
-      <c r="I20" s="32">
+      <c r="I20" s="24">
         <f>SUM('[1]1'!I20,'[1]2'!I20,'[1]3'!I20,'[1]4'!I20,'[1]5'!I20,'[1]6'!I20,'[1]7'!I20,'[1]8'!I20,'[1]9'!I20,'[1]10'!I20,'[1]11'!I20,'[1]12'!I20,'[1]13'!I20,'[1]14'!I20)</f>
         <v>2410234.4789999989</v>
       </c>
-      <c r="J20" s="32">
+      <c r="J20" s="24">
         <f>SUM('[1]1'!J20,'[1]2'!J20,'[1]3'!J20,'[1]4'!J20,'[1]5'!J20,'[1]6'!J20,'[1]7'!J20,'[1]8'!J20,'[1]9'!J20,'[1]10'!J20,'[1]11'!J20,'[1]12'!J20,'[1]13'!J20,'[1]14'!J20)</f>
         <v>2093465.3829999994</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="34">
+      <c r="B21" s="26">
         <v>175271.78400000031</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="26">
         <v>175271.78400000031</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="26">
         <v>175271.78400000031</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="26">
         <v>175271.78400000031</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="26">
         <v>175271.78400000031</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="26">
         <v>175271.78400000031</v>
       </c>
-      <c r="H21" s="34">
+      <c r="H21" s="26">
         <v>175271.78400000031</v>
       </c>
-      <c r="I21" s="34">
+      <c r="I21" s="26">
         <v>175271.78400000031</v>
       </c>
-      <c r="J21" s="34">
+      <c r="J21" s="26">
         <v>175271.78400000031</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="35" t="s">
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="20">
         <f>SUM(B23:B26)</f>
         <v>83692685.287200019</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="20">
         <f t="shared" ref="C22:J22" si="2">SUM(C23:C26)</f>
         <v>85749786.725999996</v>
       </c>
-      <c r="D22" s="28">
+      <c r="D22" s="20">
         <f t="shared" si="2"/>
         <v>87428283.76700002</v>
       </c>
-      <c r="E22" s="28">
+      <c r="E22" s="20">
         <f t="shared" si="2"/>
         <v>89504291.164000005</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="20">
         <f t="shared" si="2"/>
         <v>90504036.020999983</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G22" s="20">
         <f t="shared" si="2"/>
         <v>89880458.037</v>
       </c>
-      <c r="H22" s="28">
+      <c r="H22" s="20">
         <f t="shared" si="2"/>
         <v>85600359.985000014</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="20">
         <f t="shared" si="2"/>
         <v>89407400.268999994</v>
       </c>
-      <c r="J22" s="28">
+      <c r="J22" s="20">
         <f t="shared" si="2"/>
         <v>86438348.878999993</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="29" t="s">
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="22">
         <f>SUM('[1]1'!B23,'[1]2'!B23,'[1]3'!B23,'[1]4'!B23,'[1]5'!B23,'[1]6'!B23,'[1]7'!B23,'[1]8'!B23,'[1]9'!B23,'[1]10'!B23,'[1]11'!B23,'[1]12'!B23,'[1]13'!B23,'[1]14'!B23)</f>
         <v>2127337.4332000064</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="22">
         <f>SUM('[1]1'!C23,'[1]2'!C23,'[1]3'!C23,'[1]4'!C23,'[1]5'!C23,'[1]6'!C23,'[1]7'!C23,'[1]8'!C23,'[1]9'!C23,'[1]10'!C23,'[1]11'!C23,'[1]12'!C23,'[1]13'!C23,'[1]14'!C23)</f>
         <v>2267283.8052999997</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="22">
         <f>SUM('[1]1'!D23,'[1]2'!D23,'[1]3'!D23,'[1]4'!D23,'[1]5'!D23,'[1]6'!D23,'[1]7'!D23,'[1]8'!D23,'[1]9'!D23,'[1]10'!D23,'[1]11'!D23,'[1]12'!D23,'[1]13'!D23,'[1]14'!D23)</f>
         <v>2134217.0910000028</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="22">
         <f>SUM('[1]1'!E23,'[1]2'!E23,'[1]3'!E23,'[1]4'!E23,'[1]5'!E23,'[1]6'!E23,'[1]7'!E23,'[1]8'!E23,'[1]9'!E23,'[1]10'!E23,'[1]11'!E23,'[1]12'!E23,'[1]13'!E23,'[1]14'!E23)</f>
         <v>2196908.1889999988</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="22">
         <f>SUM('[1]1'!F23,'[1]2'!F23,'[1]3'!F23,'[1]4'!F23,'[1]5'!F23,'[1]6'!F23,'[1]7'!F23,'[1]8'!F23,'[1]9'!F23,'[1]10'!F23,'[1]11'!F23,'[1]12'!F23,'[1]13'!F23,'[1]14'!F23)</f>
         <v>2341593.3519999906</v>
       </c>
-      <c r="G23" s="30">
+      <c r="G23" s="22">
         <f>SUM('[1]1'!G23,'[1]2'!G23,'[1]3'!G23,'[1]4'!G23,'[1]5'!G23,'[1]6'!G23,'[1]7'!G23,'[1]8'!G23,'[1]9'!G23,'[1]10'!G23,'[1]11'!G23,'[1]12'!G23,'[1]13'!G23,'[1]14'!G23)</f>
         <v>2287753.2830000049</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="22">
         <f>SUM('[1]1'!H23,'[1]2'!H23,'[1]3'!H23,'[1]4'!H23,'[1]5'!H23,'[1]6'!H23,'[1]7'!H23,'[1]8'!H23,'[1]9'!H23,'[1]10'!H23,'[1]11'!H23,'[1]12'!H23,'[1]13'!H23,'[1]14'!H23)</f>
         <v>2237268.6660000025</v>
       </c>
-      <c r="I23" s="30">
+      <c r="I23" s="22">
         <f>SUM('[1]1'!I23,'[1]2'!I23,'[1]3'!I23,'[1]4'!I23,'[1]5'!I23,'[1]6'!I23,'[1]7'!I23,'[1]8'!I23,'[1]9'!I23,'[1]10'!I23,'[1]11'!I23,'[1]12'!I23,'[1]13'!I23,'[1]14'!I23)</f>
         <v>2152218.2770000058</v>
       </c>
-      <c r="J23" s="30">
+      <c r="J23" s="22">
         <f>SUM('[1]1'!J23,'[1]2'!J23,'[1]3'!J23,'[1]4'!J23,'[1]5'!J23,'[1]6'!J23,'[1]7'!J23,'[1]8'!J23,'[1]9'!J23,'[1]10'!J23,'[1]11'!J23,'[1]12'!J23,'[1]13'!J23,'[1]14'!J23)</f>
         <v>2298347.8590000044</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="31" t="s">
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="24">
         <f>SUM('[1]1'!B24,'[1]2'!B24,'[1]3'!B24,'[1]4'!B24,'[1]5'!B24,'[1]6'!B24,'[1]7'!B24,'[1]8'!B24,'[1]9'!B24,'[1]10'!B24,'[1]11'!B24,'[1]12'!B24,'[1]13'!B24,'[1]14'!B24)</f>
         <v>51711804.641000003</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="24">
         <f>SUM('[1]1'!C24,'[1]2'!C24,'[1]3'!C24,'[1]4'!C24,'[1]5'!C24,'[1]6'!C24,'[1]7'!C24,'[1]8'!C24,'[1]9'!C24,'[1]10'!C24,'[1]11'!C24,'[1]12'!C24,'[1]13'!C24,'[1]14'!C24)</f>
         <v>52832048.140700005</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="24">
         <f>SUM('[1]1'!D24,'[1]2'!D24,'[1]3'!D24,'[1]4'!D24,'[1]5'!D24,'[1]6'!D24,'[1]7'!D24,'[1]8'!D24,'[1]9'!D24,'[1]10'!D24,'[1]11'!D24,'[1]12'!D24,'[1]13'!D24,'[1]14'!D24)</f>
         <v>54070256.658000007</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="24">
         <f>SUM('[1]1'!E24,'[1]2'!E24,'[1]3'!E24,'[1]4'!E24,'[1]5'!E24,'[1]6'!E24,'[1]7'!E24,'[1]8'!E24,'[1]9'!E24,'[1]10'!E24,'[1]11'!E24,'[1]12'!E24,'[1]13'!E24,'[1]14'!E24)</f>
         <v>55313849.449000008</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="24">
         <f>SUM('[1]1'!F24,'[1]2'!F24,'[1]3'!F24,'[1]4'!F24,'[1]5'!F24,'[1]6'!F24,'[1]7'!F24,'[1]8'!F24,'[1]9'!F24,'[1]10'!F24,'[1]11'!F24,'[1]12'!F24,'[1]13'!F24,'[1]14'!F24)</f>
         <v>55637976.018999994</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="24">
         <f>SUM('[1]1'!G24,'[1]2'!G24,'[1]3'!G24,'[1]4'!G24,'[1]5'!G24,'[1]6'!G24,'[1]7'!G24,'[1]8'!G24,'[1]9'!G24,'[1]10'!G24,'[1]11'!G24,'[1]12'!G24,'[1]13'!G24,'[1]14'!G24)</f>
         <v>55434528.254000001</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="24">
         <f>SUM('[1]1'!H24,'[1]2'!H24,'[1]3'!H24,'[1]4'!H24,'[1]5'!H24,'[1]6'!H24,'[1]7'!H24,'[1]8'!H24,'[1]9'!H24,'[1]10'!H24,'[1]11'!H24,'[1]12'!H24,'[1]13'!H24,'[1]14'!H24)</f>
         <v>53562499.383000001</v>
       </c>
-      <c r="I24" s="32">
+      <c r="I24" s="24">
         <f>SUM('[1]1'!I24,'[1]2'!I24,'[1]3'!I24,'[1]4'!I24,'[1]5'!I24,'[1]6'!I24,'[1]7'!I24,'[1]8'!I24,'[1]9'!I24,'[1]10'!I24,'[1]11'!I24,'[1]12'!I24,'[1]13'!I24,'[1]14'!I24)</f>
         <v>56131919.887999989</v>
       </c>
-      <c r="J24" s="32">
+      <c r="J24" s="24">
         <f>SUM('[1]1'!J24,'[1]2'!J24,'[1]3'!J24,'[1]4'!J24,'[1]5'!J24,'[1]6'!J24,'[1]7'!J24,'[1]8'!J24,'[1]9'!J24,'[1]10'!J24,'[1]11'!J24,'[1]12'!J24,'[1]13'!J24,'[1]14'!J24)</f>
         <v>53790227.082999997</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="31" t="s">
+    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="32">
+      <c r="B25" s="24">
         <f>SUM('[1]1'!B25,'[1]2'!B25,'[1]3'!B25,'[1]4'!B25,'[1]5'!B25,'[1]6'!B25,'[1]7'!B25,'[1]8'!B25,'[1]9'!B25,'[1]10'!B25,'[1]11'!B25,'[1]12'!B25,'[1]13'!B25,'[1]14'!B25)</f>
         <v>7266068.9100000001</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="24">
         <f>SUM('[1]1'!C25,'[1]2'!C25,'[1]3'!C25,'[1]4'!C25,'[1]5'!C25,'[1]6'!C25,'[1]7'!C25,'[1]8'!C25,'[1]9'!C25,'[1]10'!C25,'[1]11'!C25,'[1]12'!C25,'[1]13'!C25,'[1]14'!C25)</f>
         <v>7296391.6309999991</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="24">
         <f>SUM('[1]1'!D25,'[1]2'!D25,'[1]3'!D25,'[1]4'!D25,'[1]5'!D25,'[1]6'!D25,'[1]7'!D25,'[1]8'!D25,'[1]9'!D25,'[1]10'!D25,'[1]11'!D25,'[1]12'!D25,'[1]13'!D25,'[1]14'!D25)</f>
         <v>7616394.2520000003</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="24">
         <f>SUM('[1]1'!E25,'[1]2'!E25,'[1]3'!E25,'[1]4'!E25,'[1]5'!E25,'[1]6'!E25,'[1]7'!E25,'[1]8'!E25,'[1]9'!E25,'[1]10'!E25,'[1]11'!E25,'[1]12'!E25,'[1]13'!E25,'[1]14'!E25)</f>
         <v>7821773.1399999997</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="24">
         <f>SUM('[1]1'!F25,'[1]2'!F25,'[1]3'!F25,'[1]4'!F25,'[1]5'!F25,'[1]6'!F25,'[1]7'!F25,'[1]8'!F25,'[1]9'!F25,'[1]10'!F25,'[1]11'!F25,'[1]12'!F25,'[1]13'!F25,'[1]14'!F25)</f>
         <v>7897845.3990000002</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="24">
         <f>SUM('[1]1'!G25,'[1]2'!G25,'[1]3'!G25,'[1]4'!G25,'[1]5'!G25,'[1]6'!G25,'[1]7'!G25,'[1]8'!G25,'[1]9'!G25,'[1]10'!G25,'[1]11'!G25,'[1]12'!G25,'[1]13'!G25,'[1]14'!G25)</f>
         <v>7921729.199</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="24">
         <f>SUM('[1]1'!H25,'[1]2'!H25,'[1]3'!H25,'[1]4'!H25,'[1]5'!H25,'[1]6'!H25,'[1]7'!H25,'[1]8'!H25,'[1]9'!H25,'[1]10'!H25,'[1]11'!H25,'[1]12'!H25,'[1]13'!H25,'[1]14'!H25)</f>
         <v>7397863.8550000014</v>
       </c>
-      <c r="I25" s="32">
+      <c r="I25" s="24">
         <f>SUM('[1]1'!I25,'[1]2'!I25,'[1]3'!I25,'[1]4'!I25,'[1]5'!I25,'[1]6'!I25,'[1]7'!I25,'[1]8'!I25,'[1]9'!I25,'[1]10'!I25,'[1]11'!I25,'[1]12'!I25,'[1]13'!I25,'[1]14'!I25)</f>
         <v>7736262.8210000005</v>
       </c>
-      <c r="J25" s="32">
+      <c r="J25" s="24">
         <f>SUM('[1]1'!J25,'[1]2'!J25,'[1]3'!J25,'[1]4'!J25,'[1]5'!J25,'[1]6'!J25,'[1]7'!J25,'[1]8'!J25,'[1]9'!J25,'[1]10'!J25,'[1]11'!J25,'[1]12'!J25,'[1]13'!J25,'[1]14'!J25)</f>
         <v>7307437.6159999985</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="33" t="s">
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="34">
+      <c r="B26" s="26">
         <f>SUM('[1]1'!B26,'[1]2'!B26,'[1]3'!B26,'[1]4'!B26,'[1]5'!B26,'[1]6'!B26,'[1]7'!B26,'[1]8'!B26,'[1]9'!B26,'[1]10'!B26,'[1]11'!B26,'[1]12'!B26,'[1]13'!B26,'[1]14'!B26)</f>
         <v>22587474.302999999</v>
       </c>
-      <c r="C26" s="34">
+      <c r="C26" s="26">
         <f>SUM('[1]1'!C26,'[1]2'!C26,'[1]3'!C26,'[1]4'!C26,'[1]5'!C26,'[1]6'!C26,'[1]7'!C26,'[1]8'!C26,'[1]9'!C26,'[1]10'!C26,'[1]11'!C26,'[1]12'!C26,'[1]13'!C26,'[1]14'!C26)</f>
         <v>23354063.149</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="26">
         <f>SUM('[1]1'!D26,'[1]2'!D26,'[1]3'!D26,'[1]4'!D26,'[1]5'!D26,'[1]6'!D26,'[1]7'!D26,'[1]8'!D26,'[1]9'!D26,'[1]10'!D26,'[1]11'!D26,'[1]12'!D26,'[1]13'!D26,'[1]14'!D26)</f>
         <v>23607415.766000003</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="26">
         <f>SUM('[1]1'!E26,'[1]2'!E26,'[1]3'!E26,'[1]4'!E26,'[1]5'!E26,'[1]6'!E26,'[1]7'!E26,'[1]8'!E26,'[1]9'!E26,'[1]10'!E26,'[1]11'!E26,'[1]12'!E26,'[1]13'!E26,'[1]14'!E26)</f>
         <v>24171760.385999996</v>
       </c>
-      <c r="F26" s="34">
+      <c r="F26" s="26">
         <f>SUM('[1]1'!F26,'[1]2'!F26,'[1]3'!F26,'[1]4'!F26,'[1]5'!F26,'[1]6'!F26,'[1]7'!F26,'[1]8'!F26,'[1]9'!F26,'[1]10'!F26,'[1]11'!F26,'[1]12'!F26,'[1]13'!F26,'[1]14'!F26)</f>
         <v>24626621.251000002</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="26">
         <f>SUM('[1]1'!G26,'[1]2'!G26,'[1]3'!G26,'[1]4'!G26,'[1]5'!G26,'[1]6'!G26,'[1]7'!G26,'[1]8'!G26,'[1]9'!G26,'[1]10'!G26,'[1]11'!G26,'[1]12'!G26,'[1]13'!G26,'[1]14'!G26)</f>
         <v>24236447.300999999</v>
       </c>
-      <c r="H26" s="34">
+      <c r="H26" s="26">
         <f>SUM('[1]1'!H26,'[1]2'!H26,'[1]3'!H26,'[1]4'!H26,'[1]5'!H26,'[1]6'!H26,'[1]7'!H26,'[1]8'!H26,'[1]9'!H26,'[1]10'!H26,'[1]11'!H26,'[1]12'!H26,'[1]13'!H26,'[1]14'!H26)</f>
         <v>22402728.081000008</v>
       </c>
-      <c r="I26" s="34">
+      <c r="I26" s="26">
         <f>SUM('[1]1'!I26,'[1]2'!I26,'[1]3'!I26,'[1]4'!I26,'[1]5'!I26,'[1]6'!I26,'[1]7'!I26,'[1]8'!I26,'[1]9'!I26,'[1]10'!I26,'[1]11'!I26,'[1]12'!I26,'[1]13'!I26,'[1]14'!I26)</f>
         <v>23386999.282999996</v>
       </c>
-      <c r="J26" s="34">
+      <c r="J26" s="26">
         <f>SUM('[1]1'!J26,'[1]2'!J26,'[1]3'!J26,'[1]4'!J26,'[1]5'!J26,'[1]6'!J26,'[1]7'!J26,'[1]8'!J26,'[1]9'!J26,'[1]10'!J26,'[1]11'!J26,'[1]12'!J26,'[1]13'!J26,'[1]14'!J26)</f>
         <v>23042336.320999995</v>
       </c>
@@ -9879,992 +9879,992 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="10"/>
-      <c r="B1" s="11">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="33"/>
+      <c r="B1" s="32">
         <v>2014</v>
       </c>
-      <c r="C1" s="11">
+      <c r="C1" s="32">
         <v>2015</v>
       </c>
-      <c r="D1" s="11">
+      <c r="D1" s="32">
         <v>2016</v>
       </c>
-      <c r="E1" s="11">
+      <c r="E1" s="32">
         <v>2017</v>
       </c>
-      <c r="F1" s="11">
+      <c r="F1" s="32">
         <v>2018</v>
       </c>
-      <c r="G1" s="11">
+      <c r="G1" s="32">
         <v>2019</v>
       </c>
-      <c r="H1" s="11">
+      <c r="H1" s="32">
         <v>2020</v>
       </c>
-      <c r="I1" s="11">
+      <c r="I1" s="32">
         <v>2021</v>
       </c>
-      <c r="J1" s="11">
+      <c r="J1" s="32">
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="13"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="35"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="11">
         <f>SUM(B5:B12)</f>
         <v>41526.830519999996</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="11">
         <f t="shared" ref="C4:J4" si="0">SUM(C5:C12)</f>
         <v>41394.85727</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <f t="shared" si="0"/>
         <v>41656.134439999994</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f t="shared" si="0"/>
         <v>42202.377619999999</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="11">
         <f t="shared" si="0"/>
         <v>42226.42164</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="11">
         <f t="shared" si="0"/>
         <v>41620.061159999997</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="11">
         <f t="shared" si="0"/>
         <v>40337.964950000001</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="11">
         <f t="shared" si="0"/>
         <v>39328.085370000001</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="11">
         <f t="shared" si="0"/>
         <v>39172.853230000001</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="13">
         <f>SUM('[1]1'!B5,'[1]2'!B5,'[1]3'!B5,'[1]4'!B5,'[1]5'!B5,'[1]6'!B5,'[1]7'!B5,'[1]8'!B5,'[1]9'!B5,'[1]10'!B5,'[1]11'!B5,'[1]12'!B5,'[1]13'!B5,'[1]14'!B5)</f>
         <v>0</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="13">
         <f>SUM('[1]1'!C5,'[1]2'!C5,'[1]3'!C5,'[1]4'!C5,'[1]5'!C5,'[1]6'!C5,'[1]7'!C5,'[1]8'!C5,'[1]9'!C5,'[1]10'!C5,'[1]11'!C5,'[1]12'!C5,'[1]13'!C5,'[1]14'!C5)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="13">
         <f>SUM('[1]1'!D5,'[1]2'!D5,'[1]3'!D5,'[1]4'!D5,'[1]5'!D5,'[1]6'!D5,'[1]7'!D5,'[1]8'!D5,'[1]9'!D5,'[1]10'!D5,'[1]11'!D5,'[1]12'!D5,'[1]13'!D5,'[1]14'!D5)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="13">
         <f>SUM('[1]1'!E5,'[1]2'!E5,'[1]3'!E5,'[1]4'!E5,'[1]5'!E5,'[1]6'!E5,'[1]7'!E5,'[1]8'!E5,'[1]9'!E5,'[1]10'!E5,'[1]11'!E5,'[1]12'!E5,'[1]13'!E5,'[1]14'!E5)</f>
         <v>0</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="13">
         <f>SUM('[1]1'!F5,'[1]2'!F5,'[1]3'!F5,'[1]4'!F5,'[1]5'!F5,'[1]6'!F5,'[1]7'!F5,'[1]8'!F5,'[1]9'!F5,'[1]10'!F5,'[1]11'!F5,'[1]12'!F5,'[1]13'!F5,'[1]14'!F5)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="13">
         <f>SUM('[1]1'!G5,'[1]2'!G5,'[1]3'!G5,'[1]4'!G5,'[1]5'!G5,'[1]6'!G5,'[1]7'!G5,'[1]8'!G5,'[1]9'!G5,'[1]10'!G5,'[1]11'!G5,'[1]12'!G5,'[1]13'!G5,'[1]14'!G5)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="13">
         <f>SUM('[1]1'!H5,'[1]2'!H5,'[1]3'!H5,'[1]4'!H5,'[1]5'!H5,'[1]6'!H5,'[1]7'!H5,'[1]8'!H5,'[1]9'!H5,'[1]10'!H5,'[1]11'!H5,'[1]12'!H5,'[1]13'!H5,'[1]14'!H5)</f>
         <v>0</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="13">
         <f>SUM('[1]1'!I5,'[1]2'!I5,'[1]3'!I5,'[1]4'!I5,'[1]5'!I5,'[1]6'!I5,'[1]7'!I5,'[1]8'!I5,'[1]9'!I5,'[1]10'!I5,'[1]11'!I5,'[1]12'!I5,'[1]13'!I5,'[1]14'!I5)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="13">
         <f>SUM('[1]1'!J5,'[1]2'!J5,'[1]3'!J5,'[1]4'!J5,'[1]5'!J5,'[1]6'!J5,'[1]7'!J5,'[1]8'!J5,'[1]9'!J5,'[1]10'!J5,'[1]11'!J5,'[1]12'!J5,'[1]13'!J5,'[1]14'!J5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="15">
         <f>SUM('[1]1'!B6,'[1]2'!B6,'[1]3'!B6,'[1]4'!B6,'[1]5'!B6,'[1]6'!B6,'[1]7'!B6,'[1]8'!B6,'[1]9'!B6,'[1]10'!B6,'[1]11'!B6,'[1]12'!B6,'[1]13'!B6,'[1]14'!B6)</f>
         <v>21940.907919999994</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="15">
         <f>SUM('[1]1'!C6,'[1]2'!C6,'[1]3'!C6,'[1]4'!C6,'[1]5'!C6,'[1]6'!C6,'[1]7'!C6,'[1]8'!C6,'[1]9'!C6,'[1]10'!C6,'[1]11'!C6,'[1]12'!C6,'[1]13'!C6,'[1]14'!C6)</f>
         <v>21877.646769999999</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="15">
         <f>SUM('[1]1'!D6,'[1]2'!D6,'[1]3'!D6,'[1]4'!D6,'[1]5'!D6,'[1]6'!D6,'[1]7'!D6,'[1]8'!D6,'[1]9'!D6,'[1]10'!D6,'[1]11'!D6,'[1]12'!D6,'[1]13'!D6,'[1]14'!D6)</f>
         <v>22006.976839999996</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="15">
         <f>SUM('[1]1'!E6,'[1]2'!E6,'[1]3'!E6,'[1]4'!E6,'[1]5'!E6,'[1]6'!E6,'[1]7'!E6,'[1]8'!E6,'[1]9'!E6,'[1]10'!E6,'[1]11'!E6,'[1]12'!E6,'[1]13'!E6,'[1]14'!E6)</f>
         <v>22293.605519999994</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="15">
         <f>SUM('[1]1'!F6,'[1]2'!F6,'[1]3'!F6,'[1]4'!F6,'[1]5'!F6,'[1]6'!F6,'[1]7'!F6,'[1]8'!F6,'[1]9'!F6,'[1]10'!F6,'[1]11'!F6,'[1]12'!F6,'[1]13'!F6,'[1]14'!F6)</f>
         <v>22302.55024</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="15">
         <f>SUM('[1]1'!G6,'[1]2'!G6,'[1]3'!G6,'[1]4'!G6,'[1]5'!G6,'[1]6'!G6,'[1]7'!G6,'[1]8'!G6,'[1]9'!G6,'[1]10'!G6,'[1]11'!G6,'[1]12'!G6,'[1]13'!G6,'[1]14'!G6)</f>
         <v>22014.280070000001</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="15">
         <f>SUM('[1]1'!H6,'[1]2'!H6,'[1]3'!H6,'[1]4'!H6,'[1]5'!H6,'[1]6'!H6,'[1]7'!H6,'[1]8'!H6,'[1]9'!H6,'[1]10'!H6,'[1]11'!H6,'[1]12'!H6,'[1]13'!H6,'[1]14'!H6)</f>
         <v>21378.455119999995</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="15">
         <f>SUM('[1]1'!I6,'[1]2'!I6,'[1]3'!I6,'[1]4'!I6,'[1]5'!I6,'[1]6'!I6,'[1]7'!I6,'[1]8'!I6,'[1]9'!I6,'[1]10'!I6,'[1]11'!I6,'[1]12'!I6,'[1]13'!I6,'[1]14'!I6)</f>
         <v>20877.60744</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="15">
         <f>SUM('[1]1'!J6,'[1]2'!J6,'[1]3'!J6,'[1]4'!J6,'[1]5'!J6,'[1]6'!J6,'[1]7'!J6,'[1]8'!J6,'[1]9'!J6,'[1]10'!J6,'[1]11'!J6,'[1]12'!J6,'[1]13'!J6,'[1]14'!J6)</f>
         <v>20806.162549999997</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="15">
         <f>SUM('[1]1'!B7,'[1]2'!B7,'[1]3'!B7,'[1]4'!B7,'[1]5'!B7,'[1]6'!B7,'[1]7'!B7,'[1]8'!B7,'[1]9'!B7,'[1]10'!B7,'[1]11'!B7,'[1]12'!B7,'[1]13'!B7,'[1]14'!B7)</f>
         <v>4290</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="15">
         <f>SUM('[1]1'!C7,'[1]2'!C7,'[1]3'!C7,'[1]4'!C7,'[1]5'!C7,'[1]6'!C7,'[1]7'!C7,'[1]8'!C7,'[1]9'!C7,'[1]10'!C7,'[1]11'!C7,'[1]12'!C7,'[1]13'!C7,'[1]14'!C7)</f>
         <v>4290</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="15">
         <f>SUM('[1]1'!D7,'[1]2'!D7,'[1]3'!D7,'[1]4'!D7,'[1]5'!D7,'[1]6'!D7,'[1]7'!D7,'[1]8'!D7,'[1]9'!D7,'[1]10'!D7,'[1]11'!D7,'[1]12'!D7,'[1]13'!D7,'[1]14'!D7)</f>
         <v>4290</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="15">
         <f>SUM('[1]1'!E7,'[1]2'!E7,'[1]3'!E7,'[1]4'!E7,'[1]5'!E7,'[1]6'!E7,'[1]7'!E7,'[1]8'!E7,'[1]9'!E7,'[1]10'!E7,'[1]11'!E7,'[1]12'!E7,'[1]13'!E7,'[1]14'!E7)</f>
         <v>4290</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="15">
         <f>SUM('[1]1'!F7,'[1]2'!F7,'[1]3'!F7,'[1]4'!F7,'[1]5'!F7,'[1]6'!F7,'[1]7'!F7,'[1]8'!F7,'[1]9'!F7,'[1]10'!F7,'[1]11'!F7,'[1]12'!F7,'[1]13'!F7,'[1]14'!F7)</f>
         <v>4290</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="15">
         <f>SUM('[1]1'!G7,'[1]2'!G7,'[1]3'!G7,'[1]4'!G7,'[1]5'!G7,'[1]6'!G7,'[1]7'!G7,'[1]8'!G7,'[1]9'!G7,'[1]10'!G7,'[1]11'!G7,'[1]12'!G7,'[1]13'!G7,'[1]14'!G7)</f>
         <v>4290</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="15">
         <f>SUM('[1]1'!H7,'[1]2'!H7,'[1]3'!H7,'[1]4'!H7,'[1]5'!H7,'[1]6'!H7,'[1]7'!H7,'[1]8'!H7,'[1]9'!H7,'[1]10'!H7,'[1]11'!H7,'[1]12'!H7,'[1]13'!H7,'[1]14'!H7)</f>
         <v>4290</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="15">
         <f>SUM('[1]1'!I7,'[1]2'!I7,'[1]3'!I7,'[1]4'!I7,'[1]5'!I7,'[1]6'!I7,'[1]7'!I7,'[1]8'!I7,'[1]9'!I7,'[1]10'!I7,'[1]11'!I7,'[1]12'!I7,'[1]13'!I7,'[1]14'!I7)</f>
         <v>4290</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="15">
         <f>SUM('[1]1'!J7,'[1]2'!J7,'[1]3'!J7,'[1]4'!J7,'[1]5'!J7,'[1]6'!J7,'[1]7'!J7,'[1]8'!J7,'[1]9'!J7,'[1]10'!J7,'[1]11'!J7,'[1]12'!J7,'[1]13'!J7,'[1]14'!J7)</f>
         <v>4290</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="15">
         <f>SUM('[1]1'!B8,'[1]2'!B8,'[1]3'!B8,'[1]4'!B8,'[1]5'!B8,'[1]6'!B8,'[1]7'!B8,'[1]8'!B8,'[1]9'!B8,'[1]10'!B8,'[1]11'!B8,'[1]12'!B8,'[1]13'!B8,'[1]14'!B8)</f>
         <v>10836.704400000001</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="15">
         <f>SUM('[1]1'!C8,'[1]2'!C8,'[1]3'!C8,'[1]4'!C8,'[1]5'!C8,'[1]6'!C8,'[1]7'!C8,'[1]8'!C8,'[1]9'!C8,'[1]10'!C8,'[1]11'!C8,'[1]12'!C8,'[1]13'!C8,'[1]14'!C8)</f>
         <v>10741.852000000001</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="15">
         <f>SUM('[1]1'!D8,'[1]2'!D8,'[1]3'!D8,'[1]4'!D8,'[1]5'!D8,'[1]6'!D8,'[1]7'!D8,'[1]8'!D8,'[1]9'!D8,'[1]10'!D8,'[1]11'!D8,'[1]12'!D8,'[1]13'!D8,'[1]14'!D8)</f>
         <v>10849.975000000002</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="15">
         <f>SUM('[1]1'!E8,'[1]2'!E8,'[1]3'!E8,'[1]4'!E8,'[1]5'!E8,'[1]6'!E8,'[1]7'!E8,'[1]8'!E8,'[1]9'!E8,'[1]10'!E8,'[1]11'!E8,'[1]12'!E8,'[1]13'!E8,'[1]14'!E8)</f>
         <v>11075.524000000001</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="15">
         <f>SUM('[1]1'!F8,'[1]2'!F8,'[1]3'!F8,'[1]4'!F8,'[1]5'!F8,'[1]6'!F8,'[1]7'!F8,'[1]8'!F8,'[1]9'!F8,'[1]10'!F8,'[1]11'!F8,'[1]12'!F8,'[1]13'!F8,'[1]14'!F8)</f>
         <v>11075.442000000001</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="15">
         <f>SUM('[1]1'!G8,'[1]2'!G8,'[1]3'!G8,'[1]4'!G8,'[1]5'!G8,'[1]6'!G8,'[1]7'!G8,'[1]8'!G8,'[1]9'!G8,'[1]10'!G8,'[1]11'!G8,'[1]12'!G8,'[1]13'!G8,'[1]14'!G8)</f>
         <v>10729.869000000001</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="15">
         <f>SUM('[1]1'!H8,'[1]2'!H8,'[1]3'!H8,'[1]4'!H8,'[1]5'!H8,'[1]6'!H8,'[1]7'!H8,'[1]8'!H8,'[1]9'!H8,'[1]10'!H8,'[1]11'!H8,'[1]12'!H8,'[1]13'!H8,'[1]14'!H8)</f>
         <v>10058.848</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="15">
         <f>SUM('[1]1'!I8,'[1]2'!I8,'[1]3'!I8,'[1]4'!I8,'[1]5'!I8,'[1]6'!I8,'[1]7'!I8,'[1]8'!I8,'[1]9'!I8,'[1]10'!I8,'[1]11'!I8,'[1]12'!I8,'[1]13'!I8,'[1]14'!I8)</f>
         <v>9527.6949999999997</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="15">
         <f>SUM('[1]1'!J8,'[1]2'!J8,'[1]3'!J8,'[1]4'!J8,'[1]5'!J8,'[1]6'!J8,'[1]7'!J8,'[1]8'!J8,'[1]9'!J8,'[1]10'!J8,'[1]11'!J8,'[1]12'!J8,'[1]13'!J8,'[1]14'!J8)</f>
         <v>9415.8970000000008</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="15">
         <f>SUM('[1]1'!B9,'[1]2'!B9,'[1]3'!B9,'[1]4'!B9,'[1]5'!B9,'[1]6'!B9,'[1]7'!B9,'[1]8'!B9,'[1]9'!B9,'[1]10'!B9,'[1]11'!B9,'[1]12'!B9,'[1]13'!B9,'[1]14'!B9)</f>
         <v>1363</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="15">
         <f>SUM('[1]1'!C9,'[1]2'!C9,'[1]3'!C9,'[1]4'!C9,'[1]5'!C9,'[1]6'!C9,'[1]7'!C9,'[1]8'!C9,'[1]9'!C9,'[1]10'!C9,'[1]11'!C9,'[1]12'!C9,'[1]13'!C9,'[1]14'!C9)</f>
         <v>1363.3150000000001</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="15">
         <f>SUM('[1]1'!D9,'[1]2'!D9,'[1]3'!D9,'[1]4'!D9,'[1]5'!D9,'[1]6'!D9,'[1]7'!D9,'[1]8'!D9,'[1]9'!D9,'[1]10'!D9,'[1]11'!D9,'[1]12'!D9,'[1]13'!D9,'[1]14'!D9)</f>
         <v>1363.5</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="15">
         <f>SUM('[1]1'!E9,'[1]2'!E9,'[1]3'!E9,'[1]4'!E9,'[1]5'!E9,'[1]6'!E9,'[1]7'!E9,'[1]8'!E9,'[1]9'!E9,'[1]10'!E9,'[1]11'!E9,'[1]12'!E9,'[1]13'!E9,'[1]14'!E9)</f>
         <v>1363.5</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="15">
         <f>SUM('[1]1'!F9,'[1]2'!F9,'[1]3'!F9,'[1]4'!F9,'[1]5'!F9,'[1]6'!F9,'[1]7'!F9,'[1]8'!F9,'[1]9'!F9,'[1]10'!F9,'[1]11'!F9,'[1]12'!F9,'[1]13'!F9,'[1]14'!F9)</f>
         <v>1363.5</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="15">
         <f>SUM('[1]1'!G9,'[1]2'!G9,'[1]3'!G9,'[1]4'!G9,'[1]5'!G9,'[1]6'!G9,'[1]7'!G9,'[1]8'!G9,'[1]9'!G9,'[1]10'!G9,'[1]11'!G9,'[1]12'!G9,'[1]13'!G9,'[1]14'!G9)</f>
         <v>1363.5</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="15">
         <f>SUM('[1]1'!H9,'[1]2'!H9,'[1]3'!H9,'[1]4'!H9,'[1]5'!H9,'[1]6'!H9,'[1]7'!H9,'[1]8'!H9,'[1]9'!H9,'[1]10'!H9,'[1]11'!H9,'[1]12'!H9,'[1]13'!H9,'[1]14'!H9)</f>
         <v>1363.5</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="15">
         <f>SUM('[1]1'!I9,'[1]2'!I9,'[1]3'!I9,'[1]4'!I9,'[1]5'!I9,'[1]6'!I9,'[1]7'!I9,'[1]8'!I9,'[1]9'!I9,'[1]10'!I9,'[1]11'!I9,'[1]12'!I9,'[1]13'!I9,'[1]14'!I9)</f>
         <v>1363.5</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="15">
         <f>SUM('[1]1'!J9,'[1]2'!J9,'[1]3'!J9,'[1]4'!J9,'[1]5'!J9,'[1]6'!J9,'[1]7'!J9,'[1]8'!J9,'[1]9'!J9,'[1]10'!J9,'[1]11'!J9,'[1]12'!J9,'[1]13'!J9,'[1]14'!J9)</f>
         <v>1363.5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="15">
         <f>SUM('[1]1'!B10,'[1]2'!B10,'[1]3'!B10,'[1]4'!B10,'[1]5'!B10,'[1]6'!B10,'[1]7'!B10,'[1]8'!B10,'[1]9'!B10,'[1]10'!B10,'[1]11'!B10,'[1]12'!B10,'[1]13'!B10,'[1]14'!B10)</f>
         <v>833.66899999999998</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="15">
         <f>SUM('[1]1'!C10,'[1]2'!C10,'[1]3'!C10,'[1]4'!C10,'[1]5'!C10,'[1]6'!C10,'[1]7'!C10,'[1]8'!C10,'[1]9'!C10,'[1]10'!C10,'[1]11'!C10,'[1]12'!C10,'[1]13'!C10,'[1]14'!C10)</f>
         <v>855.5630000000001</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="15">
         <f>SUM('[1]1'!D10,'[1]2'!D10,'[1]3'!D10,'[1]4'!D10,'[1]5'!D10,'[1]6'!D10,'[1]7'!D10,'[1]8'!D10,'[1]9'!D10,'[1]10'!D10,'[1]11'!D10,'[1]12'!D10,'[1]13'!D10,'[1]14'!D10)</f>
         <v>873.99199999999996</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="15">
         <f>SUM('[1]1'!E10,'[1]2'!E10,'[1]3'!E10,'[1]4'!E10,'[1]5'!E10,'[1]6'!E10,'[1]7'!E10,'[1]8'!E10,'[1]9'!E10,'[1]10'!E10,'[1]11'!E10,'[1]12'!E10,'[1]13'!E10,'[1]14'!E10)</f>
         <v>895.98699999999985</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="15">
         <f>SUM('[1]1'!F10,'[1]2'!F10,'[1]3'!F10,'[1]4'!F10,'[1]5'!F10,'[1]6'!F10,'[1]7'!F10,'[1]8'!F10,'[1]9'!F10,'[1]10'!F10,'[1]11'!F10,'[1]12'!F10,'[1]13'!F10,'[1]14'!F10)</f>
         <v>910.90980000000002</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="15">
         <f>SUM('[1]1'!G10,'[1]2'!G10,'[1]3'!G10,'[1]4'!G10,'[1]5'!G10,'[1]6'!G10,'[1]7'!G10,'[1]8'!G10,'[1]9'!G10,'[1]10'!G10,'[1]11'!G10,'[1]12'!G10,'[1]13'!G10,'[1]14'!G10)</f>
         <v>937.70399999999995</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="15">
         <f>SUM('[1]1'!H10,'[1]2'!H10,'[1]3'!H10,'[1]4'!H10,'[1]5'!H10,'[1]6'!H10,'[1]7'!H10,'[1]8'!H10,'[1]9'!H10,'[1]10'!H10,'[1]11'!H10,'[1]12'!H10,'[1]13'!H10,'[1]14'!H10)</f>
         <v>961.74929999999995</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="15">
         <f>SUM('[1]1'!I10,'[1]2'!I10,'[1]3'!I10,'[1]4'!I10,'[1]5'!I10,'[1]6'!I10,'[1]7'!I10,'[1]8'!I10,'[1]9'!I10,'[1]10'!I10,'[1]11'!I10,'[1]12'!I10,'[1]13'!I10,'[1]14'!I10)</f>
         <v>983.15179999999987</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="15">
         <f>SUM('[1]1'!J10,'[1]2'!J10,'[1]3'!J10,'[1]4'!J10,'[1]5'!J10,'[1]6'!J10,'[1]7'!J10,'[1]8'!J10,'[1]9'!J10,'[1]10'!J10,'[1]11'!J10,'[1]12'!J10,'[1]13'!J10,'[1]14'!J10)</f>
         <v>1012.2180000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="15">
         <f>SUM('[1]1'!B11,'[1]2'!B11,'[1]3'!B11,'[1]4'!B11,'[1]5'!B11,'[1]6'!B11,'[1]7'!B11,'[1]8'!B11,'[1]9'!B11,'[1]10'!B11,'[1]11'!B11,'[1]12'!B11,'[1]13'!B11,'[1]14'!B11)</f>
         <v>1091.0491999999999</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="15">
         <f>SUM('[1]1'!C11,'[1]2'!C11,'[1]3'!C11,'[1]4'!C11,'[1]5'!C11,'[1]6'!C11,'[1]7'!C11,'[1]8'!C11,'[1]9'!C11,'[1]10'!C11,'[1]11'!C11,'[1]12'!C11,'[1]13'!C11,'[1]14'!C11)</f>
         <v>1094.9804999999999</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="15">
         <f>SUM('[1]1'!D11,'[1]2'!D11,'[1]3'!D11,'[1]4'!D11,'[1]5'!D11,'[1]6'!D11,'[1]7'!D11,'[1]8'!D11,'[1]9'!D11,'[1]10'!D11,'[1]11'!D11,'[1]12'!D11,'[1]13'!D11,'[1]14'!D11)</f>
         <v>1100.1906000000001</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="15">
         <f>SUM('[1]1'!E11,'[1]2'!E11,'[1]3'!E11,'[1]4'!E11,'[1]5'!E11,'[1]6'!E11,'[1]7'!E11,'[1]8'!E11,'[1]9'!E11,'[1]10'!E11,'[1]11'!E11,'[1]12'!E11,'[1]13'!E11,'[1]14'!E11)</f>
         <v>1112.2610999999999</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="15">
         <f>SUM('[1]1'!F11,'[1]2'!F11,'[1]3'!F11,'[1]4'!F11,'[1]5'!F11,'[1]6'!F11,'[1]7'!F11,'[1]8'!F11,'[1]9'!F11,'[1]10'!F11,'[1]11'!F11,'[1]12'!F11,'[1]13'!F11,'[1]14'!F11)</f>
         <v>1112.5196000000003</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="15">
         <f>SUM('[1]1'!G11,'[1]2'!G11,'[1]3'!G11,'[1]4'!G11,'[1]5'!G11,'[1]6'!G11,'[1]7'!G11,'[1]8'!G11,'[1]9'!G11,'[1]10'!G11,'[1]11'!G11,'[1]12'!G11,'[1]13'!G11,'[1]14'!G11)</f>
         <v>1113.2080900000001</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="15">
         <f>SUM('[1]1'!H11,'[1]2'!H11,'[1]3'!H11,'[1]4'!H11,'[1]5'!H11,'[1]6'!H11,'[1]7'!H11,'[1]8'!H11,'[1]9'!H11,'[1]10'!H11,'[1]11'!H11,'[1]12'!H11,'[1]13'!H11,'[1]14'!H11)</f>
         <v>1113.9125300000001</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="15">
         <f>SUM('[1]1'!I11,'[1]2'!I11,'[1]3'!I11,'[1]4'!I11,'[1]5'!I11,'[1]6'!I11,'[1]7'!I11,'[1]8'!I11,'[1]9'!I11,'[1]10'!I11,'[1]11'!I11,'[1]12'!I11,'[1]13'!I11,'[1]14'!I11)</f>
         <v>1114.63113</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="15">
         <f>SUM('[1]1'!J11,'[1]2'!J11,'[1]3'!J11,'[1]4'!J11,'[1]5'!J11,'[1]6'!J11,'[1]7'!J11,'[1]8'!J11,'[1]9'!J11,'[1]10'!J11,'[1]11'!J11,'[1]12'!J11,'[1]13'!J11,'[1]14'!J11)</f>
         <v>1113.5756799999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="15">
         <f>SUM('[1]1'!B12,'[1]2'!B12,'[1]3'!B12,'[1]4'!B12,'[1]5'!B12,'[1]6'!B12,'[1]7'!B12,'[1]8'!B12,'[1]9'!B12,'[1]10'!B12,'[1]11'!B12,'[1]12'!B12,'[1]13'!B12,'[1]14'!B12)</f>
         <v>1171.5</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="15">
         <f>SUM('[1]1'!C12,'[1]2'!C12,'[1]3'!C12,'[1]4'!C12,'[1]5'!C12,'[1]6'!C12,'[1]7'!C12,'[1]8'!C12,'[1]9'!C12,'[1]10'!C12,'[1]11'!C12,'[1]12'!C12,'[1]13'!C12,'[1]14'!C12)</f>
         <v>1171.5</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="15">
         <f>SUM('[1]1'!D12,'[1]2'!D12,'[1]3'!D12,'[1]4'!D12,'[1]5'!D12,'[1]6'!D12,'[1]7'!D12,'[1]8'!D12,'[1]9'!D12,'[1]10'!D12,'[1]11'!D12,'[1]12'!D12,'[1]13'!D12,'[1]14'!D12)</f>
         <v>1171.5</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="15">
         <f>SUM('[1]1'!E12,'[1]2'!E12,'[1]3'!E12,'[1]4'!E12,'[1]5'!E12,'[1]6'!E12,'[1]7'!E12,'[1]8'!E12,'[1]9'!E12,'[1]10'!E12,'[1]11'!E12,'[1]12'!E12,'[1]13'!E12,'[1]14'!E12)</f>
         <v>1171.5</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="15">
         <f>SUM('[1]1'!F12,'[1]2'!F12,'[1]3'!F12,'[1]4'!F12,'[1]5'!F12,'[1]6'!F12,'[1]7'!F12,'[1]8'!F12,'[1]9'!F12,'[1]10'!F12,'[1]11'!F12,'[1]12'!F12,'[1]13'!F12,'[1]14'!F12)</f>
         <v>1171.5</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="15">
         <f>SUM('[1]1'!G12,'[1]2'!G12,'[1]3'!G12,'[1]4'!G12,'[1]5'!G12,'[1]6'!G12,'[1]7'!G12,'[1]8'!G12,'[1]9'!G12,'[1]10'!G12,'[1]11'!G12,'[1]12'!G12,'[1]13'!G12,'[1]14'!G12)</f>
         <v>1171.5</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="15">
         <f>SUM('[1]1'!H12,'[1]2'!H12,'[1]3'!H12,'[1]4'!H12,'[1]5'!H12,'[1]6'!H12,'[1]7'!H12,'[1]8'!H12,'[1]9'!H12,'[1]10'!H12,'[1]11'!H12,'[1]12'!H12,'[1]13'!H12,'[1]14'!H12)</f>
         <v>1171.5</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="15">
         <f>SUM('[1]1'!I12,'[1]2'!I12,'[1]3'!I12,'[1]4'!I12,'[1]5'!I12,'[1]6'!I12,'[1]7'!I12,'[1]8'!I12,'[1]9'!I12,'[1]10'!I12,'[1]11'!I12,'[1]12'!I12,'[1]13'!I12,'[1]14'!I12)</f>
         <v>1171.5</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="15">
         <f>SUM('[1]1'!J12,'[1]2'!J12,'[1]3'!J12,'[1]4'!J12,'[1]5'!J12,'[1]6'!J12,'[1]7'!J12,'[1]8'!J12,'[1]9'!J12,'[1]10'!J12,'[1]11'!J12,'[1]12'!J12,'[1]13'!J12,'[1]14'!J12)</f>
         <v>1171.5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="11">
         <f>SUM(B14:B21)</f>
         <v>168548927.22962007</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="11">
         <f t="shared" ref="C13:J13" si="1">SUM(C14:C21)</f>
         <v>163849009.58366999</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="11">
         <f t="shared" si="1"/>
         <v>162955887.10934007</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="11">
         <f t="shared" si="1"/>
         <v>170301522.83002001</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="11">
         <f t="shared" si="1"/>
         <v>172180583.21744001</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="11">
         <f t="shared" si="1"/>
         <v>170005369.50658002</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="11">
         <f t="shared" si="1"/>
         <v>158839720.47188997</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="11">
         <f t="shared" si="1"/>
         <v>166028084.29711002</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="11">
         <f t="shared" si="1"/>
         <v>165254240.03297001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="13">
         <f>SUM('[1]1'!B14,'[1]2'!B14,'[1]3'!B14,'[1]4'!B14,'[1]5'!B14,'[1]6'!B14,'[1]7'!B14,'[1]8'!B14,'[1]9'!B14,'[1]10'!B14,'[1]11'!B14,'[1]12'!B14,'[1]13'!B14,'[1]14'!B14)</f>
         <v>2076.7944199999956</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="13">
         <f>SUM('[1]1'!C14,'[1]2'!C14,'[1]3'!C14,'[1]4'!C14,'[1]5'!C14,'[1]6'!C14,'[1]7'!C14,'[1]8'!C14,'[1]9'!C14,'[1]10'!C14,'[1]11'!C14,'[1]12'!C14,'[1]13'!C14,'[1]14'!C14)</f>
         <v>2078.2503699999952</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="13">
         <f>SUM('[1]1'!D14,'[1]2'!D14,'[1]3'!D14,'[1]4'!D14,'[1]5'!D14,'[1]6'!D14,'[1]7'!D14,'[1]8'!D14,'[1]9'!D14,'[1]10'!D14,'[1]11'!D14,'[1]12'!D14,'[1]13'!D14,'[1]14'!D14)</f>
         <v>2075.6643399999962</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="13">
         <f>SUM('[1]1'!E14,'[1]2'!E14,'[1]3'!E14,'[1]4'!E14,'[1]5'!E14,'[1]6'!E14,'[1]7'!E14,'[1]8'!E14,'[1]9'!E14,'[1]10'!E14,'[1]11'!E14,'[1]12'!E14,'[1]13'!E14,'[1]14'!E14)</f>
         <v>2076.6260199999956</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="13">
         <f>SUM('[1]1'!F14,'[1]2'!F14,'[1]3'!F14,'[1]4'!F14,'[1]5'!F14,'[1]6'!F14,'[1]7'!F14,'[1]8'!F14,'[1]9'!F14,'[1]10'!F14,'[1]11'!F14,'[1]12'!F14,'[1]13'!F14,'[1]14'!F14)</f>
         <v>2061.9714399999957</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="13">
         <f>SUM('[1]1'!G14,'[1]2'!G14,'[1]3'!G14,'[1]4'!G14,'[1]5'!G14,'[1]6'!G14,'[1]7'!G14,'[1]8'!G14,'[1]9'!G14,'[1]10'!G14,'[1]11'!G14,'[1]12'!G14,'[1]13'!G14,'[1]14'!G14)</f>
         <v>2069.0745799999959</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="13">
         <f>SUM('[1]1'!H14,'[1]2'!H14,'[1]3'!H14,'[1]4'!H14,'[1]5'!H14,'[1]6'!H14,'[1]7'!H14,'[1]8'!H14,'[1]9'!H14,'[1]10'!H14,'[1]11'!H14,'[1]12'!H14,'[1]13'!H14,'[1]14'!H14)</f>
         <v>2079.5208899999966</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="13">
         <f>SUM('[1]1'!I14,'[1]2'!I14,'[1]3'!I14,'[1]4'!I14,'[1]5'!I14,'[1]6'!I14,'[1]7'!I14,'[1]8'!I14,'[1]9'!I14,'[1]10'!I14,'[1]11'!I14,'[1]12'!I14,'[1]13'!I14,'[1]14'!I14)</f>
         <v>2087.7051099999958</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="13">
         <f>SUM('[1]1'!J14,'[1]2'!J14,'[1]3'!J14,'[1]4'!J14,'[1]5'!J14,'[1]6'!J14,'[1]7'!J14,'[1]8'!J14,'[1]9'!J14,'[1]10'!J14,'[1]11'!J14,'[1]12'!J14,'[1]13'!J14,'[1]14'!J14)</f>
         <v>2100.3769699999957</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="15">
         <f>SUM('[1]1'!B15,'[1]2'!B15,'[1]3'!B15,'[1]4'!B15,'[1]5'!B15,'[1]6'!B15,'[1]7'!B15,'[1]8'!B15,'[1]9'!B15,'[1]10'!B15,'[1]11'!B15,'[1]12'!B15,'[1]13'!B15,'[1]14'!B15)</f>
         <v>86013493.427200034</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="15">
         <f>SUM('[1]1'!C15,'[1]2'!C15,'[1]3'!C15,'[1]4'!C15,'[1]5'!C15,'[1]6'!C15,'[1]7'!C15,'[1]8'!C15,'[1]9'!C15,'[1]10'!C15,'[1]11'!C15,'[1]12'!C15,'[1]13'!C15,'[1]14'!C15)</f>
         <v>83893758.431299984</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="15">
         <f>SUM('[1]1'!D15,'[1]2'!D15,'[1]3'!D15,'[1]4'!D15,'[1]5'!D15,'[1]6'!D15,'[1]7'!D15,'[1]8'!D15,'[1]9'!D15,'[1]10'!D15,'[1]11'!D15,'[1]12'!D15,'[1]13'!D15,'[1]14'!D15)</f>
         <v>83305632.317000017</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="15">
         <f>SUM('[1]1'!E15,'[1]2'!E15,'[1]3'!E15,'[1]4'!E15,'[1]5'!E15,'[1]6'!E15,'[1]7'!E15,'[1]8'!E15,'[1]9'!E15,'[1]10'!E15,'[1]11'!E15,'[1]12'!E15,'[1]13'!E15,'[1]14'!E15)</f>
         <v>87041288.026999995</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="15">
         <f>SUM('[1]1'!F15,'[1]2'!F15,'[1]3'!F15,'[1]4'!F15,'[1]5'!F15,'[1]6'!F15,'[1]7'!F15,'[1]8'!F15,'[1]9'!F15,'[1]10'!F15,'[1]11'!F15,'[1]12'!F15,'[1]13'!F15,'[1]14'!F15)</f>
         <v>88002380.354999989</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="15">
         <f>SUM('[1]1'!G15,'[1]2'!G15,'[1]3'!G15,'[1]4'!G15,'[1]5'!G15,'[1]6'!G15,'[1]7'!G15,'[1]8'!G15,'[1]9'!G15,'[1]10'!G15,'[1]11'!G15,'[1]12'!G15,'[1]13'!G15,'[1]14'!G15)</f>
         <v>86991236.566000015</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="15">
         <f>SUM('[1]1'!H15,'[1]2'!H15,'[1]3'!H15,'[1]4'!H15,'[1]5'!H15,'[1]6'!H15,'[1]7'!H15,'[1]8'!H15,'[1]9'!H15,'[1]10'!H15,'[1]11'!H15,'[1]12'!H15,'[1]13'!H15,'[1]14'!H15)</f>
         <v>81445899.992999986</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="15">
         <f>SUM('[1]1'!I15,'[1]2'!I15,'[1]3'!I15,'[1]4'!I15,'[1]5'!I15,'[1]6'!I15,'[1]7'!I15,'[1]8'!I15,'[1]9'!I15,'[1]10'!I15,'[1]11'!I15,'[1]12'!I15,'[1]13'!I15,'[1]14'!I15)</f>
         <v>84907950.802000001</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="15">
         <f>SUM('[1]1'!J15,'[1]2'!J15,'[1]3'!J15,'[1]4'!J15,'[1]5'!J15,'[1]6'!J15,'[1]7'!J15,'[1]8'!J15,'[1]9'!J15,'[1]10'!J15,'[1]11'!J15,'[1]12'!J15,'[1]13'!J15,'[1]14'!J15)</f>
         <v>84503127.281000003</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="15">
         <f>SUM('[1]1'!B16,'[1]2'!B16,'[1]3'!B16,'[1]4'!B16,'[1]5'!B16,'[1]6'!B16,'[1]7'!B16,'[1]8'!B16,'[1]9'!B16,'[1]10'!B16,'[1]11'!B16,'[1]12'!B16,'[1]13'!B16,'[1]14'!B16)</f>
         <v>30324873.359999999</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="15">
         <f>SUM('[1]1'!C16,'[1]2'!C16,'[1]3'!C16,'[1]4'!C16,'[1]5'!C16,'[1]6'!C16,'[1]7'!C16,'[1]8'!C16,'[1]9'!C16,'[1]10'!C16,'[1]11'!C16,'[1]12'!C16,'[1]13'!C16,'[1]14'!C16)</f>
         <v>26840847.649999999</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="15">
         <f>SUM('[1]1'!D16,'[1]2'!D16,'[1]3'!D16,'[1]4'!D16,'[1]5'!D16,'[1]6'!D16,'[1]7'!D16,'[1]8'!D16,'[1]9'!D16,'[1]10'!D16,'[1]11'!D16,'[1]12'!D16,'[1]13'!D16,'[1]14'!D16)</f>
         <v>24104222.150000002</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="15">
         <f>SUM('[1]1'!E16,'[1]2'!E16,'[1]3'!E16,'[1]4'!E16,'[1]5'!E16,'[1]6'!E16,'[1]7'!E16,'[1]8'!E16,'[1]9'!E16,'[1]10'!E16,'[1]11'!E16,'[1]12'!E16,'[1]13'!E16,'[1]14'!E16)</f>
         <v>28339577.039999999</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="15">
         <f>SUM('[1]1'!F16,'[1]2'!F16,'[1]3'!F16,'[1]4'!F16,'[1]5'!F16,'[1]6'!F16,'[1]7'!F16,'[1]8'!F16,'[1]9'!F16,'[1]10'!F16,'[1]11'!F16,'[1]12'!F16,'[1]13'!F16,'[1]14'!F16)</f>
         <v>29921311.170000002</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="15">
         <f>SUM('[1]1'!G16,'[1]2'!G16,'[1]3'!G16,'[1]4'!G16,'[1]5'!G16,'[1]6'!G16,'[1]7'!G16,'[1]8'!G16,'[1]9'!G16,'[1]10'!G16,'[1]11'!G16,'[1]12'!G16,'[1]13'!G16,'[1]14'!G16)</f>
         <v>30246208.84</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="15">
         <f>SUM('[1]1'!H16,'[1]2'!H16,'[1]3'!H16,'[1]4'!H16,'[1]5'!H16,'[1]6'!H16,'[1]7'!H16,'[1]8'!H16,'[1]9'!H16,'[1]10'!H16,'[1]11'!H16,'[1]12'!H16,'[1]13'!H16,'[1]14'!H16)</f>
         <v>30043279.77</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="15">
         <f>SUM('[1]1'!I16,'[1]2'!I16,'[1]3'!I16,'[1]4'!I16,'[1]5'!I16,'[1]6'!I16,'[1]7'!I16,'[1]8'!I16,'[1]9'!I16,'[1]10'!I16,'[1]11'!I16,'[1]12'!I16,'[1]13'!I16,'[1]14'!I16)</f>
         <v>30731180.379999999</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="15">
         <f>SUM('[1]1'!J16,'[1]2'!J16,'[1]3'!J16,'[1]4'!J16,'[1]5'!J16,'[1]6'!J16,'[1]7'!J16,'[1]8'!J16,'[1]9'!J16,'[1]10'!J16,'[1]11'!J16,'[1]12'!J16,'[1]13'!J16,'[1]14'!J16)</f>
         <v>31021810.439999998</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="15">
         <f>SUM('[1]1'!B17,'[1]2'!B17,'[1]3'!B17,'[1]4'!B17,'[1]5'!B17,'[1]6'!B17,'[1]7'!B17,'[1]8'!B17,'[1]9'!B17,'[1]10'!B17,'[1]11'!B17,'[1]12'!B17,'[1]13'!B17,'[1]14'!B17)</f>
         <v>44420480.449000016</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="15">
         <f>SUM('[1]1'!C17,'[1]2'!C17,'[1]3'!C17,'[1]4'!C17,'[1]5'!C17,'[1]6'!C17,'[1]7'!C17,'[1]8'!C17,'[1]9'!C17,'[1]10'!C17,'[1]11'!C17,'[1]12'!C17,'[1]13'!C17,'[1]14'!C17)</f>
         <v>44819831.069999985</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="15">
         <f>SUM('[1]1'!D17,'[1]2'!D17,'[1]3'!D17,'[1]4'!D17,'[1]5'!D17,'[1]6'!D17,'[1]7'!D17,'[1]8'!D17,'[1]9'!D17,'[1]10'!D17,'[1]11'!D17,'[1]12'!D17,'[1]13'!D17,'[1]14'!D17)</f>
         <v>45704070.480000004</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="15">
         <f>SUM('[1]1'!E17,'[1]2'!E17,'[1]3'!E17,'[1]4'!E17,'[1]5'!E17,'[1]6'!E17,'[1]7'!E17,'[1]8'!E17,'[1]9'!E17,'[1]10'!E17,'[1]11'!E17,'[1]12'!E17,'[1]13'!E17,'[1]14'!E17)</f>
         <v>45431680.267999992</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="15">
         <f>SUM('[1]1'!F17,'[1]2'!F17,'[1]3'!F17,'[1]4'!F17,'[1]5'!F17,'[1]6'!F17,'[1]7'!F17,'[1]8'!F17,'[1]9'!F17,'[1]10'!F17,'[1]11'!F17,'[1]12'!F17,'[1]13'!F17,'[1]14'!F17)</f>
         <v>45070754.584000006</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="15">
         <f>SUM('[1]1'!G17,'[1]2'!G17,'[1]3'!G17,'[1]4'!G17,'[1]5'!G17,'[1]6'!G17,'[1]7'!G17,'[1]8'!G17,'[1]9'!G17,'[1]10'!G17,'[1]11'!G17,'[1]12'!G17,'[1]13'!G17,'[1]14'!G17)</f>
         <v>41386690.89199999</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="15">
         <f>SUM('[1]1'!H17,'[1]2'!H17,'[1]3'!H17,'[1]4'!H17,'[1]5'!H17,'[1]6'!H17,'[1]7'!H17,'[1]8'!H17,'[1]9'!H17,'[1]10'!H17,'[1]11'!H17,'[1]12'!H17,'[1]13'!H17,'[1]14'!H17)</f>
         <v>35198100.92899999</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="15">
         <f>SUM('[1]1'!I17,'[1]2'!I17,'[1]3'!I17,'[1]4'!I17,'[1]5'!I17,'[1]6'!I17,'[1]7'!I17,'[1]8'!I17,'[1]9'!I17,'[1]10'!I17,'[1]11'!I17,'[1]12'!I17,'[1]13'!I17,'[1]14'!I17)</f>
         <v>38631451.995999992</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="15">
         <f>SUM('[1]1'!J17,'[1]2'!J17,'[1]3'!J17,'[1]4'!J17,'[1]5'!J17,'[1]6'!J17,'[1]7'!J17,'[1]8'!J17,'[1]9'!J17,'[1]10'!J17,'[1]11'!J17,'[1]12'!J17,'[1]13'!J17,'[1]14'!J17)</f>
         <v>41017314.489</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="15">
         <f>SUM('[1]1'!B18,'[1]2'!B18,'[1]3'!B18,'[1]4'!B18,'[1]5'!B18,'[1]6'!B18,'[1]7'!B18,'[1]8'!B18,'[1]9'!B18,'[1]10'!B18,'[1]11'!B18,'[1]12'!B18,'[1]13'!B18,'[1]14'!B18)</f>
         <v>2204674.9</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="15">
         <f>SUM('[1]1'!C18,'[1]2'!C18,'[1]3'!C18,'[1]4'!C18,'[1]5'!C18,'[1]6'!C18,'[1]7'!C18,'[1]8'!C18,'[1]9'!C18,'[1]10'!C18,'[1]11'!C18,'[1]12'!C18,'[1]13'!C18,'[1]14'!C18)</f>
         <v>2749023.0999999996</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="15">
         <f>SUM('[1]1'!D18,'[1]2'!D18,'[1]3'!D18,'[1]4'!D18,'[1]5'!D18,'[1]6'!D18,'[1]7'!D18,'[1]8'!D18,'[1]9'!D18,'[1]10'!D18,'[1]11'!D18,'[1]12'!D18,'[1]13'!D18,'[1]14'!D18)</f>
         <v>4049243.6780000003</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="15">
         <f>SUM('[1]1'!E18,'[1]2'!E18,'[1]3'!E18,'[1]4'!E18,'[1]5'!E18,'[1]6'!E18,'[1]7'!E18,'[1]8'!E18,'[1]9'!E18,'[1]10'!E18,'[1]11'!E18,'[1]12'!E18,'[1]13'!E18,'[1]14'!E18)</f>
         <v>3722405.4339999999</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="15">
         <f>SUM('[1]1'!F18,'[1]2'!F18,'[1]3'!F18,'[1]4'!F18,'[1]5'!F18,'[1]6'!F18,'[1]7'!F18,'[1]8'!F18,'[1]9'!F18,'[1]10'!F18,'[1]11'!F18,'[1]12'!F18,'[1]13'!F18,'[1]14'!F18)</f>
         <v>3690871.87</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="15">
         <f>SUM('[1]1'!G18,'[1]2'!G18,'[1]3'!G18,'[1]4'!G18,'[1]5'!G18,'[1]6'!G18,'[1]7'!G18,'[1]8'!G18,'[1]9'!G18,'[1]10'!G18,'[1]11'!G18,'[1]12'!G18,'[1]13'!G18,'[1]14'!G18)</f>
         <v>5518520.6710000001</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="15">
         <f>SUM('[1]1'!H18,'[1]2'!H18,'[1]3'!H18,'[1]4'!H18,'[1]5'!H18,'[1]6'!H18,'[1]7'!H18,'[1]8'!H18,'[1]9'!H18,'[1]10'!H18,'[1]11'!H18,'[1]12'!H18,'[1]13'!H18,'[1]14'!H18)</f>
         <v>6041267.5499999989</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="15">
         <f>SUM('[1]1'!I18,'[1]2'!I18,'[1]3'!I18,'[1]4'!I18,'[1]5'!I18,'[1]6'!I18,'[1]7'!I18,'[1]8'!I18,'[1]9'!I18,'[1]10'!I18,'[1]11'!I18,'[1]12'!I18,'[1]13'!I18,'[1]14'!I18)</f>
         <v>5239842.1099999994</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="15">
         <f>SUM('[1]1'!J18,'[1]2'!J18,'[1]3'!J18,'[1]4'!J18,'[1]5'!J18,'[1]6'!J18,'[1]7'!J18,'[1]8'!J18,'[1]9'!J18,'[1]10'!J18,'[1]11'!J18,'[1]12'!J18,'[1]13'!J18,'[1]14'!J18)</f>
         <v>2533599.0180000002</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="15">
         <f>SUM('[1]1'!B19,'[1]2'!B19,'[1]3'!B19,'[1]4'!B19,'[1]5'!B19,'[1]6'!B19,'[1]7'!B19,'[1]8'!B19,'[1]9'!B19,'[1]10'!B19,'[1]11'!B19,'[1]12'!B19,'[1]13'!B19,'[1]14'!B19)</f>
         <v>3498294.1009999998</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="15">
         <f>SUM('[1]1'!C19,'[1]2'!C19,'[1]3'!C19,'[1]4'!C19,'[1]5'!C19,'[1]6'!C19,'[1]7'!C19,'[1]8'!C19,'[1]9'!C19,'[1]10'!C19,'[1]11'!C19,'[1]12'!C19,'[1]13'!C19,'[1]14'!C19)</f>
         <v>3572812.2869999981</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="15">
         <f>SUM('[1]1'!D19,'[1]2'!D19,'[1]3'!D19,'[1]4'!D19,'[1]5'!D19,'[1]6'!D19,'[1]7'!D19,'[1]8'!D19,'[1]9'!D19,'[1]10'!D19,'[1]11'!D19,'[1]12'!D19,'[1]13'!D19,'[1]14'!D19)</f>
         <v>3613882.0269999984</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="15">
         <f>SUM('[1]1'!E19,'[1]2'!E19,'[1]3'!E19,'[1]4'!E19,'[1]5'!E19,'[1]6'!E19,'[1]7'!E19,'[1]8'!E19,'[1]9'!E19,'[1]10'!E19,'[1]11'!E19,'[1]12'!E19,'[1]13'!E19,'[1]14'!E19)</f>
         <v>3719689.5779999997</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="15">
         <f>SUM('[1]1'!F19,'[1]2'!F19,'[1]3'!F19,'[1]4'!F19,'[1]5'!F19,'[1]6'!F19,'[1]7'!F19,'[1]8'!F19,'[1]9'!F19,'[1]10'!F19,'[1]11'!F19,'[1]12'!F19,'[1]13'!F19,'[1]14'!F19)</f>
         <v>3690413.1099999994</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="15">
         <f>SUM('[1]1'!G19,'[1]2'!G19,'[1]3'!G19,'[1]4'!G19,'[1]5'!G19,'[1]6'!G19,'[1]7'!G19,'[1]8'!G19,'[1]9'!G19,'[1]10'!G19,'[1]11'!G19,'[1]12'!G19,'[1]13'!G19,'[1]14'!G19)</f>
         <v>3676697.149999999</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="15">
         <f>SUM('[1]1'!H19,'[1]2'!H19,'[1]3'!H19,'[1]4'!H19,'[1]5'!H19,'[1]6'!H19,'[1]7'!H19,'[1]8'!H19,'[1]9'!H19,'[1]10'!H19,'[1]11'!H19,'[1]12'!H19,'[1]13'!H19,'[1]14'!H19)</f>
         <v>3789565.7849999978</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="15">
         <f>SUM('[1]1'!I19,'[1]2'!I19,'[1]3'!I19,'[1]4'!I19,'[1]5'!I19,'[1]6'!I19,'[1]7'!I19,'[1]8'!I19,'[1]9'!I19,'[1]10'!I19,'[1]11'!I19,'[1]12'!I19,'[1]13'!I19,'[1]14'!I19)</f>
         <v>3930065.0409999988</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="15">
         <f>SUM('[1]1'!J19,'[1]2'!J19,'[1]3'!J19,'[1]4'!J19,'[1]5'!J19,'[1]6'!J19,'[1]7'!J19,'[1]8'!J19,'[1]9'!J19,'[1]10'!J19,'[1]11'!J19,'[1]12'!J19,'[1]13'!J19,'[1]14'!J19)</f>
         <v>3907551.2609999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="15">
         <f>SUM('[1]1'!B20,'[1]2'!B20,'[1]3'!B20,'[1]4'!B20,'[1]5'!B20,'[1]6'!B20,'[1]7'!B20,'[1]8'!B20,'[1]9'!B20,'[1]10'!B20,'[1]11'!B20,'[1]12'!B20,'[1]13'!B20,'[1]14'!B20)</f>
         <v>1909762.4139999999</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="15">
         <f>SUM('[1]1'!C20,'[1]2'!C20,'[1]3'!C20,'[1]4'!C20,'[1]5'!C20,'[1]6'!C20,'[1]7'!C20,'[1]8'!C20,'[1]9'!C20,'[1]10'!C20,'[1]11'!C20,'[1]12'!C20,'[1]13'!C20,'[1]14'!C20)</f>
         <v>1795387.0110000004</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="15">
         <f>SUM('[1]1'!D20,'[1]2'!D20,'[1]3'!D20,'[1]4'!D20,'[1]5'!D20,'[1]6'!D20,'[1]7'!D20,'[1]8'!D20,'[1]9'!D20,'[1]10'!D20,'[1]11'!D20,'[1]12'!D20,'[1]13'!D20,'[1]14'!D20)</f>
         <v>2001489.0090000003</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="15">
         <f>SUM('[1]1'!E20,'[1]2'!E20,'[1]3'!E20,'[1]4'!E20,'[1]5'!E20,'[1]6'!E20,'[1]7'!E20,'[1]8'!E20,'[1]9'!E20,'[1]10'!E20,'[1]11'!E20,'[1]12'!E20,'[1]13'!E20,'[1]14'!E20)</f>
         <v>1869534.0729999996</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="15">
         <f>SUM('[1]1'!F20,'[1]2'!F20,'[1]3'!F20,'[1]4'!F20,'[1]5'!F20,'[1]6'!F20,'[1]7'!F20,'[1]8'!F20,'[1]9'!F20,'[1]10'!F20,'[1]11'!F20,'[1]12'!F20,'[1]13'!F20,'[1]14'!F20)</f>
         <v>1627518.3729999997</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="15">
         <f>SUM('[1]1'!G20,'[1]2'!G20,'[1]3'!G20,'[1]4'!G20,'[1]5'!G20,'[1]6'!G20,'[1]7'!G20,'[1]8'!G20,'[1]9'!G20,'[1]10'!G20,'[1]11'!G20,'[1]12'!G20,'[1]13'!G20,'[1]14'!G20)</f>
         <v>2008674.5289999996</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="15">
         <f>SUM('[1]1'!H20,'[1]2'!H20,'[1]3'!H20,'[1]4'!H20,'[1]5'!H20,'[1]6'!H20,'[1]7'!H20,'[1]8'!H20,'[1]9'!H20,'[1]10'!H20,'[1]11'!H20,'[1]12'!H20,'[1]13'!H20,'[1]14'!H20)</f>
         <v>2144255.1399999997</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="15">
         <f>SUM('[1]1'!I20,'[1]2'!I20,'[1]3'!I20,'[1]4'!I20,'[1]5'!I20,'[1]6'!I20,'[1]7'!I20,'[1]8'!I20,'[1]9'!I20,'[1]10'!I20,'[1]11'!I20,'[1]12'!I20,'[1]13'!I20,'[1]14'!I20)</f>
         <v>2410234.4789999989</v>
       </c>
-      <c r="J20" s="19">
+      <c r="J20" s="15">
         <f>SUM('[1]1'!J20,'[1]2'!J20,'[1]3'!J20,'[1]4'!J20,'[1]5'!J20,'[1]6'!J20,'[1]7'!J20,'[1]8'!J20,'[1]9'!J20,'[1]10'!J20,'[1]11'!J20,'[1]12'!J20,'[1]13'!J20,'[1]14'!J20)</f>
         <v>2093465.3829999994</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="17">
         <v>175271.78400000031</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="17">
         <v>175271.78400000031</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="17">
         <v>175271.78400000031</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="17">
         <v>175271.78400000031</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="17">
         <v>175271.78400000031</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="17">
         <v>175271.78400000031</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="17">
         <v>175271.78400000031</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="17">
         <v>175271.78400000031</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="17">
         <v>175271.78400000031</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="11">
         <f>SUM(B23:B26)</f>
         <v>83692685.287200019</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="11">
         <f t="shared" ref="C22:J22" si="2">SUM(C23:C26)</f>
         <v>85749786.725999996</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="11">
         <f t="shared" si="2"/>
         <v>87428283.76700002</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="11">
         <f t="shared" si="2"/>
         <v>89504291.164000005</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="11">
         <f t="shared" si="2"/>
         <v>90504036.020999983</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="11">
         <f t="shared" si="2"/>
         <v>89880458.037</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="11">
         <f t="shared" si="2"/>
         <v>85600359.985000014</v>
       </c>
-      <c r="I22" s="15">
+      <c r="I22" s="11">
         <f t="shared" si="2"/>
         <v>89407400.268999994</v>
       </c>
-      <c r="J22" s="15">
+      <c r="J22" s="11">
         <f t="shared" si="2"/>
         <v>86438348.878999993</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="13">
         <f>SUM('[1]1'!B23,'[1]2'!B23,'[1]3'!B23,'[1]4'!B23,'[1]5'!B23,'[1]6'!B23,'[1]7'!B23,'[1]8'!B23,'[1]9'!B23,'[1]10'!B23,'[1]11'!B23,'[1]12'!B23,'[1]13'!B23,'[1]14'!B23)</f>
         <v>2127337.4332000064</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="13">
         <f>SUM('[1]1'!C23,'[1]2'!C23,'[1]3'!C23,'[1]4'!C23,'[1]5'!C23,'[1]6'!C23,'[1]7'!C23,'[1]8'!C23,'[1]9'!C23,'[1]10'!C23,'[1]11'!C23,'[1]12'!C23,'[1]13'!C23,'[1]14'!C23)</f>
         <v>2267283.8052999997</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="13">
         <f>SUM('[1]1'!D23,'[1]2'!D23,'[1]3'!D23,'[1]4'!D23,'[1]5'!D23,'[1]6'!D23,'[1]7'!D23,'[1]8'!D23,'[1]9'!D23,'[1]10'!D23,'[1]11'!D23,'[1]12'!D23,'[1]13'!D23,'[1]14'!D23)</f>
         <v>2134217.0910000028</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="13">
         <f>SUM('[1]1'!E23,'[1]2'!E23,'[1]3'!E23,'[1]4'!E23,'[1]5'!E23,'[1]6'!E23,'[1]7'!E23,'[1]8'!E23,'[1]9'!E23,'[1]10'!E23,'[1]11'!E23,'[1]12'!E23,'[1]13'!E23,'[1]14'!E23)</f>
         <v>2196908.1889999988</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="13">
         <f>SUM('[1]1'!F23,'[1]2'!F23,'[1]3'!F23,'[1]4'!F23,'[1]5'!F23,'[1]6'!F23,'[1]7'!F23,'[1]8'!F23,'[1]9'!F23,'[1]10'!F23,'[1]11'!F23,'[1]12'!F23,'[1]13'!F23,'[1]14'!F23)</f>
         <v>2341593.3519999906</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="13">
         <f>SUM('[1]1'!G23,'[1]2'!G23,'[1]3'!G23,'[1]4'!G23,'[1]5'!G23,'[1]6'!G23,'[1]7'!G23,'[1]8'!G23,'[1]9'!G23,'[1]10'!G23,'[1]11'!G23,'[1]12'!G23,'[1]13'!G23,'[1]14'!G23)</f>
         <v>2287753.2830000049</v>
       </c>
-      <c r="H23" s="17">
+      <c r="H23" s="13">
         <f>SUM('[1]1'!H23,'[1]2'!H23,'[1]3'!H23,'[1]4'!H23,'[1]5'!H23,'[1]6'!H23,'[1]7'!H23,'[1]8'!H23,'[1]9'!H23,'[1]10'!H23,'[1]11'!H23,'[1]12'!H23,'[1]13'!H23,'[1]14'!H23)</f>
         <v>2237268.6660000025</v>
       </c>
-      <c r="I23" s="17">
+      <c r="I23" s="13">
         <f>SUM('[1]1'!I23,'[1]2'!I23,'[1]3'!I23,'[1]4'!I23,'[1]5'!I23,'[1]6'!I23,'[1]7'!I23,'[1]8'!I23,'[1]9'!I23,'[1]10'!I23,'[1]11'!I23,'[1]12'!I23,'[1]13'!I23,'[1]14'!I23)</f>
         <v>2152218.2770000058</v>
       </c>
-      <c r="J23" s="17">
+      <c r="J23" s="13">
         <f>SUM('[1]1'!J23,'[1]2'!J23,'[1]3'!J23,'[1]4'!J23,'[1]5'!J23,'[1]6'!J23,'[1]7'!J23,'[1]8'!J23,'[1]9'!J23,'[1]10'!J23,'[1]11'!J23,'[1]12'!J23,'[1]13'!J23,'[1]14'!J23)</f>
         <v>2298347.8590000044</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="15">
         <f>SUM('[1]1'!B24,'[1]2'!B24,'[1]3'!B24,'[1]4'!B24,'[1]5'!B24,'[1]6'!B24,'[1]7'!B24,'[1]8'!B24,'[1]9'!B24,'[1]10'!B24,'[1]11'!B24,'[1]12'!B24,'[1]13'!B24,'[1]14'!B24)</f>
         <v>51711804.641000003</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="15">
         <f>SUM('[1]1'!C24,'[1]2'!C24,'[1]3'!C24,'[1]4'!C24,'[1]5'!C24,'[1]6'!C24,'[1]7'!C24,'[1]8'!C24,'[1]9'!C24,'[1]10'!C24,'[1]11'!C24,'[1]12'!C24,'[1]13'!C24,'[1]14'!C24)</f>
         <v>52832048.140700005</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="15">
         <f>SUM('[1]1'!D24,'[1]2'!D24,'[1]3'!D24,'[1]4'!D24,'[1]5'!D24,'[1]6'!D24,'[1]7'!D24,'[1]8'!D24,'[1]9'!D24,'[1]10'!D24,'[1]11'!D24,'[1]12'!D24,'[1]13'!D24,'[1]14'!D24)</f>
         <v>54070256.658000007</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="15">
         <f>SUM('[1]1'!E24,'[1]2'!E24,'[1]3'!E24,'[1]4'!E24,'[1]5'!E24,'[1]6'!E24,'[1]7'!E24,'[1]8'!E24,'[1]9'!E24,'[1]10'!E24,'[1]11'!E24,'[1]12'!E24,'[1]13'!E24,'[1]14'!E24)</f>
         <v>55313849.449000008</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="15">
         <f>SUM('[1]1'!F24,'[1]2'!F24,'[1]3'!F24,'[1]4'!F24,'[1]5'!F24,'[1]6'!F24,'[1]7'!F24,'[1]8'!F24,'[1]9'!F24,'[1]10'!F24,'[1]11'!F24,'[1]12'!F24,'[1]13'!F24,'[1]14'!F24)</f>
         <v>55637976.018999994</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="15">
         <f>SUM('[1]1'!G24,'[1]2'!G24,'[1]3'!G24,'[1]4'!G24,'[1]5'!G24,'[1]6'!G24,'[1]7'!G24,'[1]8'!G24,'[1]9'!G24,'[1]10'!G24,'[1]11'!G24,'[1]12'!G24,'[1]13'!G24,'[1]14'!G24)</f>
         <v>55434528.254000001</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="15">
         <f>SUM('[1]1'!H24,'[1]2'!H24,'[1]3'!H24,'[1]4'!H24,'[1]5'!H24,'[1]6'!H24,'[1]7'!H24,'[1]8'!H24,'[1]9'!H24,'[1]10'!H24,'[1]11'!H24,'[1]12'!H24,'[1]13'!H24,'[1]14'!H24)</f>
         <v>53562499.383000001</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="15">
         <f>SUM('[1]1'!I24,'[1]2'!I24,'[1]3'!I24,'[1]4'!I24,'[1]5'!I24,'[1]6'!I24,'[1]7'!I24,'[1]8'!I24,'[1]9'!I24,'[1]10'!I24,'[1]11'!I24,'[1]12'!I24,'[1]13'!I24,'[1]14'!I24)</f>
         <v>56131919.887999989</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="15">
         <f>SUM('[1]1'!J24,'[1]2'!J24,'[1]3'!J24,'[1]4'!J24,'[1]5'!J24,'[1]6'!J24,'[1]7'!J24,'[1]8'!J24,'[1]9'!J24,'[1]10'!J24,'[1]11'!J24,'[1]12'!J24,'[1]13'!J24,'[1]14'!J24)</f>
         <v>53790227.082999997</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="18" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="15">
         <f>SUM('[1]1'!B25,'[1]2'!B25,'[1]3'!B25,'[1]4'!B25,'[1]5'!B25,'[1]6'!B25,'[1]7'!B25,'[1]8'!B25,'[1]9'!B25,'[1]10'!B25,'[1]11'!B25,'[1]12'!B25,'[1]13'!B25,'[1]14'!B25)</f>
         <v>7266068.9100000001</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="15">
         <f>SUM('[1]1'!C25,'[1]2'!C25,'[1]3'!C25,'[1]4'!C25,'[1]5'!C25,'[1]6'!C25,'[1]7'!C25,'[1]8'!C25,'[1]9'!C25,'[1]10'!C25,'[1]11'!C25,'[1]12'!C25,'[1]13'!C25,'[1]14'!C25)</f>
         <v>7296391.6309999991</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="15">
         <f>SUM('[1]1'!D25,'[1]2'!D25,'[1]3'!D25,'[1]4'!D25,'[1]5'!D25,'[1]6'!D25,'[1]7'!D25,'[1]8'!D25,'[1]9'!D25,'[1]10'!D25,'[1]11'!D25,'[1]12'!D25,'[1]13'!D25,'[1]14'!D25)</f>
         <v>7616394.2520000003</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="15">
         <f>SUM('[1]1'!E25,'[1]2'!E25,'[1]3'!E25,'[1]4'!E25,'[1]5'!E25,'[1]6'!E25,'[1]7'!E25,'[1]8'!E25,'[1]9'!E25,'[1]10'!E25,'[1]11'!E25,'[1]12'!E25,'[1]13'!E25,'[1]14'!E25)</f>
         <v>7821773.1399999997</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="15">
         <f>SUM('[1]1'!F25,'[1]2'!F25,'[1]3'!F25,'[1]4'!F25,'[1]5'!F25,'[1]6'!F25,'[1]7'!F25,'[1]8'!F25,'[1]9'!F25,'[1]10'!F25,'[1]11'!F25,'[1]12'!F25,'[1]13'!F25,'[1]14'!F25)</f>
         <v>7897845.3990000002</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="15">
         <f>SUM('[1]1'!G25,'[1]2'!G25,'[1]3'!G25,'[1]4'!G25,'[1]5'!G25,'[1]6'!G25,'[1]7'!G25,'[1]8'!G25,'[1]9'!G25,'[1]10'!G25,'[1]11'!G25,'[1]12'!G25,'[1]13'!G25,'[1]14'!G25)</f>
         <v>7921729.199</v>
       </c>
-      <c r="H25" s="19">
+      <c r="H25" s="15">
         <f>SUM('[1]1'!H25,'[1]2'!H25,'[1]3'!H25,'[1]4'!H25,'[1]5'!H25,'[1]6'!H25,'[1]7'!H25,'[1]8'!H25,'[1]9'!H25,'[1]10'!H25,'[1]11'!H25,'[1]12'!H25,'[1]13'!H25,'[1]14'!H25)</f>
         <v>7397863.8550000014</v>
       </c>
-      <c r="I25" s="19">
+      <c r="I25" s="15">
         <f>SUM('[1]1'!I25,'[1]2'!I25,'[1]3'!I25,'[1]4'!I25,'[1]5'!I25,'[1]6'!I25,'[1]7'!I25,'[1]8'!I25,'[1]9'!I25,'[1]10'!I25,'[1]11'!I25,'[1]12'!I25,'[1]13'!I25,'[1]14'!I25)</f>
         <v>7736262.8210000005</v>
       </c>
-      <c r="J25" s="19">
+      <c r="J25" s="15">
         <f>SUM('[1]1'!J25,'[1]2'!J25,'[1]3'!J25,'[1]4'!J25,'[1]5'!J25,'[1]6'!J25,'[1]7'!J25,'[1]8'!J25,'[1]9'!J25,'[1]10'!J25,'[1]11'!J25,'[1]12'!J25,'[1]13'!J25,'[1]14'!J25)</f>
         <v>7307437.6159999985</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="17">
         <f>SUM('[1]1'!B26,'[1]2'!B26,'[1]3'!B26,'[1]4'!B26,'[1]5'!B26,'[1]6'!B26,'[1]7'!B26,'[1]8'!B26,'[1]9'!B26,'[1]10'!B26,'[1]11'!B26,'[1]12'!B26,'[1]13'!B26,'[1]14'!B26)</f>
         <v>22587474.302999999</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="17">
         <f>SUM('[1]1'!C26,'[1]2'!C26,'[1]3'!C26,'[1]4'!C26,'[1]5'!C26,'[1]6'!C26,'[1]7'!C26,'[1]8'!C26,'[1]9'!C26,'[1]10'!C26,'[1]11'!C26,'[1]12'!C26,'[1]13'!C26,'[1]14'!C26)</f>
         <v>23354063.149</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="17">
         <f>SUM('[1]1'!D26,'[1]2'!D26,'[1]3'!D26,'[1]4'!D26,'[1]5'!D26,'[1]6'!D26,'[1]7'!D26,'[1]8'!D26,'[1]9'!D26,'[1]10'!D26,'[1]11'!D26,'[1]12'!D26,'[1]13'!D26,'[1]14'!D26)</f>
         <v>23607415.766000003</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="17">
         <f>SUM('[1]1'!E26,'[1]2'!E26,'[1]3'!E26,'[1]4'!E26,'[1]5'!E26,'[1]6'!E26,'[1]7'!E26,'[1]8'!E26,'[1]9'!E26,'[1]10'!E26,'[1]11'!E26,'[1]12'!E26,'[1]13'!E26,'[1]14'!E26)</f>
         <v>24171760.385999996</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="17">
         <f>SUM('[1]1'!F26,'[1]2'!F26,'[1]3'!F26,'[1]4'!F26,'[1]5'!F26,'[1]6'!F26,'[1]7'!F26,'[1]8'!F26,'[1]9'!F26,'[1]10'!F26,'[1]11'!F26,'[1]12'!F26,'[1]13'!F26,'[1]14'!F26)</f>
         <v>24626621.251000002</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="17">
         <f>SUM('[1]1'!G26,'[1]2'!G26,'[1]3'!G26,'[1]4'!G26,'[1]5'!G26,'[1]6'!G26,'[1]7'!G26,'[1]8'!G26,'[1]9'!G26,'[1]10'!G26,'[1]11'!G26,'[1]12'!G26,'[1]13'!G26,'[1]14'!G26)</f>
         <v>24236447.300999999</v>
       </c>
-      <c r="H26" s="21">
+      <c r="H26" s="17">
         <f>SUM('[1]1'!H26,'[1]2'!H26,'[1]3'!H26,'[1]4'!H26,'[1]5'!H26,'[1]6'!H26,'[1]7'!H26,'[1]8'!H26,'[1]9'!H26,'[1]10'!H26,'[1]11'!H26,'[1]12'!H26,'[1]13'!H26,'[1]14'!H26)</f>
         <v>22402728.081000008</v>
       </c>
-      <c r="I26" s="21">
+      <c r="I26" s="17">
         <f>SUM('[1]1'!I26,'[1]2'!I26,'[1]3'!I26,'[1]4'!I26,'[1]5'!I26,'[1]6'!I26,'[1]7'!I26,'[1]8'!I26,'[1]9'!I26,'[1]10'!I26,'[1]11'!I26,'[1]12'!I26,'[1]13'!I26,'[1]14'!I26)</f>
         <v>23386999.282999996</v>
       </c>
-      <c r="J26" s="21">
+      <c r="J26" s="17">
         <f>SUM('[1]1'!J26,'[1]2'!J26,'[1]3'!J26,'[1]4'!J26,'[1]5'!J26,'[1]6'!J26,'[1]7'!J26,'[1]8'!J26,'[1]9'!J26,'[1]10'!J26,'[1]11'!J26,'[1]12'!J26,'[1]13'!J26,'[1]14'!J26)</f>
         <v>23042336.320999995</v>
       </c>

</xml_diff>